<commit_message>
일단 커밋 from mac
</commit_message>
<xml_diff>
--- a/PIO_check/PIO_SCRATCH.xlsx
+++ b/PIO_check/PIO_SCRATCH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robomation_TUF15\Desktop\TUF15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imseongsu/robomation/personal_tjdtn/PIO_check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0E443E-D431-4EDC-8F58-03CD4589A440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F5F964-1202-BC4C-815B-EE676768F452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1965" windowWidth="23235" windowHeight="12825" xr2:uid="{385024C5-CB96-4C20-A0A9-1BB6D9BF6AC5}"/>
+    <workbookView xWindow="4240" yWindow="2280" windowWidth="28360" windowHeight="16180" xr2:uid="{385024C5-CB96-4C20-A0A9-1BB6D9BF6AC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>CMA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2만/일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>종목명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,17 +162,32 @@
     <t>15년차에 두배차이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>생활비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구독료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저축가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4달에 44만</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,14 +284,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -310,10 +324,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,13 +526,13 @@
                 <c:formatCode>#,##0.00_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>183.32</c:v>
+                  <c:v>183.43</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>428.28</c:v>
+                  <c:v>428.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>913.2</c:v>
+                  <c:v>916.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2390,22 +2410,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD9DA4A-515C-43D0-9EBA-F5949D4DBDAF}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19">
       <c r="C1" t="s">
         <v>10</v>
       </c>
@@ -2413,55 +2438,55 @@
         <v>1338.7</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:19">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="Q3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" t="s">
         <v>21</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>22</v>
       </c>
-      <c r="S3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C4">
@@ -2470,332 +2495,348 @@
       <c r="D4">
         <v>15.38</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <f>C4*D1</f>
         <v>20589.206000000002</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <f>D4*D1</f>
         <v>20589.206000000002</v>
       </c>
       <c r="Q4" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>302383</v>
       </c>
-      <c r="S4" s="8">
+      <c r="S4" s="7">
         <v>1.0123</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:19">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>178.03</v>
       </c>
-      <c r="D5" s="2">
-        <v>183.32</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="15">
+        <v>183.43</v>
+      </c>
+      <c r="E5" s="2">
         <f>D5-C5</f>
-        <v>5.289999999999992</v>
-      </c>
-      <c r="F5" s="8">
+        <v>5.4000000000000057</v>
+      </c>
+      <c r="F5" s="7">
         <f>(D5/C5-1)</f>
-        <v>2.9714093130371211E-2</v>
-      </c>
-      <c r="I5" s="6" t="s">
+        <v>3.0331966522496145E-2</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>237314</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <f>D5*D1</f>
-        <v>245410.484</v>
-      </c>
-      <c r="M5" s="7">
+        <v>245557.74100000001</v>
+      </c>
+      <c r="M5" s="6">
         <f>L5-K5</f>
-        <v>8096.4839999999967</v>
-      </c>
-      <c r="N5" s="8">
+        <v>8243.7410000000091</v>
+      </c>
+      <c r="N5" s="7">
         <f>(L5/K5-1)</f>
-        <v>3.4117178084731581E-2</v>
+        <v>3.4737693519977686E-2</v>
       </c>
       <c r="Q5" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="6">
         <v>29107</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5" s="7">
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:19">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>406.5</v>
       </c>
-      <c r="D6" s="2">
-        <v>428.28</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="15">
+        <v>428.98</v>
+      </c>
+      <c r="E6" s="2">
         <f>D6-C6</f>
-        <v>21.779999999999973</v>
-      </c>
-      <c r="F6" s="8">
+        <v>22.480000000000018</v>
+      </c>
+      <c r="F6" s="7">
         <f>(D6/C6-1)</f>
-        <v>5.357933579335783E-2</v>
-      </c>
-      <c r="I6" s="6" t="s">
+        <v>5.530135301353023E-2</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>541173</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <f>D6*D1</f>
-        <v>573338.43599999999</v>
-      </c>
-      <c r="M6" s="7">
+        <v>574275.52600000007</v>
+      </c>
+      <c r="M6" s="6">
         <f>L6-K6</f>
-        <v>32165.435999999987</v>
-      </c>
-      <c r="N6" s="8">
+        <v>33102.526000000071</v>
+      </c>
+      <c r="N6" s="7">
         <f>(L6/K6-1)</f>
-        <v>5.9436512908071837E-2</v>
+        <v>6.1168103360663029E-2</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R6" s="7">
+        <v>23</v>
+      </c>
+      <c r="R6" s="6">
         <v>-5397</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="7">
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:19">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>682</v>
       </c>
-      <c r="D7" s="2">
-        <v>913.2</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="15">
+        <v>916.56</v>
+      </c>
+      <c r="E7" s="2">
         <f>D7-C7</f>
-        <v>231.20000000000005</v>
-      </c>
-      <c r="F7" s="8">
+        <v>234.55999999999995</v>
+      </c>
+      <c r="F7" s="7">
         <f>(D7/C7-1)</f>
-        <v>0.33900293255131975</v>
-      </c>
-      <c r="I7" s="6" t="s">
+        <v>0.34392961876832828</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>912448</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f>D7*D1</f>
-        <v>1222500.8400000001</v>
-      </c>
-      <c r="M7" s="7">
+        <v>1226998.872</v>
+      </c>
+      <c r="M7" s="6">
         <f>L7-K7</f>
-        <v>310052.84000000008</v>
-      </c>
-      <c r="N7" s="8">
+        <v>314550.87199999997</v>
+      </c>
+      <c r="N7" s="7">
         <f>(L7/K7-1)</f>
-        <v>0.33980329837974343</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+        <v>0.34473292943817069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>SUM(C4:C7)</f>
         <v>1281.9099999999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f>SUM(D4:D7)</f>
-        <v>1540.18</v>
-      </c>
-      <c r="E8" s="3">
+        <v>1544.35</v>
+      </c>
+      <c r="E8" s="2">
         <f>D8-C8</f>
-        <v>258.27000000000021</v>
-      </c>
-      <c r="F8" s="8">
+        <v>262.44000000000005</v>
+      </c>
+      <c r="F8" s="7">
         <f>(D8/C8-1)</f>
-        <v>0.20147280230281406</v>
-      </c>
-      <c r="I8" s="6" t="s">
+        <v>0.20472576077883797</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <f>SUM(K4:K7)</f>
         <v>1711524.206</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <f>SUM(L4:L7)</f>
-        <v>2061838.966</v>
-      </c>
-      <c r="M8" s="7">
+        <v>2067421.345</v>
+      </c>
+      <c r="M8" s="6">
         <f>L8-K8</f>
-        <v>350314.76</v>
-      </c>
-      <c r="N8" s="8">
+        <v>355897.13899999997</v>
+      </c>
+      <c r="N8" s="7">
         <f>(L8/K8-1)</f>
-        <v>0.20467999153732097</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0.20794163340042182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="L11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="L12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" t="s">
         <v>25</v>
       </c>
-      <c r="M12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K14" s="7"/>
-      <c r="L14" s="14">
-        <f>L8</f>
-        <v>2061838.966</v>
-      </c>
-      <c r="M14" s="15">
+      <c r="N12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="K14" s="6"/>
+      <c r="L14" s="13">
+        <v>2067421</v>
+      </c>
+      <c r="M14" s="14">
         <v>45375</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="L15" s="14">
+    <row r="15" spans="1:19">
+      <c r="L15" s="13">
         <f>(L14+1000000)*1.02</f>
-        <v>3123075.7453200002</v>
-      </c>
-      <c r="M15" s="15">
+        <v>3128769.42</v>
+      </c>
+      <c r="M15" s="14">
         <v>45406</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="L16" s="14">
+    <row r="16" spans="1:19">
+      <c r="L16" s="13">
         <f t="shared" ref="L16:L18" si="0">(L15+1000000)*1.02</f>
-        <v>4205537.2602264006</v>
-      </c>
-      <c r="M16" s="15">
+        <v>4211344.8084000004</v>
+      </c>
+      <c r="M16" s="14">
         <v>45436</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L17" s="14">
+    <row r="17" spans="1:13">
+      <c r="L17" s="13">
         <f t="shared" si="0"/>
-        <v>5309648.0054309284</v>
-      </c>
-      <c r="M17" s="15">
+        <v>5315571.7045680005</v>
+      </c>
+      <c r="M17" s="14">
         <v>45467</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L18" s="14">
+    <row r="18" spans="1:13">
+      <c r="L18" s="13">
         <f t="shared" si="0"/>
-        <v>6435840.9655395467</v>
-      </c>
-      <c r="M18" s="15">
+        <v>6441883.1386593608</v>
+      </c>
+      <c r="M18" s="14">
         <v>45497</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G20" s="7">
-        <v>600000</v>
-      </c>
+    <row r="20" spans="1:13">
+      <c r="G20" s="6"/>
       <c r="J20" t="s">
         <v>19</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="16">
         <v>1643900</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:13">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+      <c r="J21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="16">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="11">
         <v>45372</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <f>SUM(C22:G22)</f>
         <v>2708698</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>2058131</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>214812</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>100981</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>30179</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>304595</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I23" t="s">
-        <v>20</v>
+      <c r="J22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="16">
+        <v>23190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="16">
+        <f>K20-K21-K22</f>
+        <v>1020710</v>
       </c>
     </row>
   </sheetData>
@@ -2829,1931 +2870,1931 @@
       <selection activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="9" style="7"/>
-    <col min="3" max="3" width="13.625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9" style="3"/>
-    <col min="5" max="6" width="9.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="12.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9" style="6"/>
+    <col min="3" max="3" width="13.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2"/>
+    <col min="5" max="6" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7">
+    <row r="1" spans="1:8">
+      <c r="A1" s="6">
         <f>F2</f>
         <v>2000000</v>
       </c>
-      <c r="C1" s="7">
+      <c r="C1" s="6">
         <v>2000000</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="6">
         <f>(A1+F2)*G2</f>
         <v>4040000</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <f>C1+F$2</f>
         <v>4000000</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>3000000</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>2000000</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>1.01</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+    <row r="3" spans="1:8">
+      <c r="A3" s="6">
         <f>(A2+F$2)*G$2</f>
         <v>6100400</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <f>C2+F$2</f>
         <v>6000000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    <row r="4" spans="1:8">
+      <c r="A4" s="6">
         <f>(A3+F$2)*G$2</f>
         <v>8181404</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <f t="shared" ref="C4:C12" si="0">C3+F$2</f>
         <v>8000000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+    <row r="5" spans="1:8">
+      <c r="A5" s="6">
         <f t="shared" ref="A5:A68" si="1">(A4+F$2)*G$2</f>
         <v>10283218.040000001</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+    <row r="6" spans="1:8">
+      <c r="A6" s="6">
         <f t="shared" si="1"/>
         <v>12406050.220400002</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>12000000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+    <row r="7" spans="1:8">
+      <c r="A7" s="6">
         <f t="shared" si="1"/>
         <v>14550110.722604003</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>14000000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    <row r="8" spans="1:8">
+      <c r="A8" s="6">
         <f t="shared" si="1"/>
         <v>16715611.829830043</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>16000000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+    <row r="9" spans="1:8">
+      <c r="A9" s="6">
         <f t="shared" si="1"/>
         <v>18902767.948128343</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>18000000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" spans="1:8">
+      <c r="A10" s="6">
         <f t="shared" si="1"/>
         <v>21111795.627609625</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>20000000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+    <row r="11" spans="1:8">
+      <c r="A11" s="6">
         <f t="shared" si="1"/>
         <v>23342913.583885722</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>22000000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+    <row r="12" spans="1:8">
+      <c r="A12" s="6">
         <f t="shared" si="1"/>
         <v>25596342.719724581</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f t="shared" si="0"/>
         <v>24000000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+    <row r="13" spans="1:8">
+      <c r="A13" s="6">
         <f t="shared" si="1"/>
         <v>27872306.146921828</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f>(C12+F$2)*D13</f>
         <v>27040000</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+    <row r="14" spans="1:8">
+      <c r="A14" s="6">
         <f t="shared" si="1"/>
         <v>30171029.208391048</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <f>C13+F$2</f>
         <v>29040000</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+    <row r="15" spans="1:8">
+      <c r="A15" s="6">
         <f t="shared" si="1"/>
         <v>32492739.50047496</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <f t="shared" ref="C15:C23" si="2">C14+F$2</f>
         <v>31040000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+    <row r="16" spans="1:8">
+      <c r="A16" s="6">
         <f t="shared" si="1"/>
         <v>34837666.895479709</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f t="shared" si="2"/>
         <v>33040000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+    <row r="17" spans="1:4">
+      <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>37206043.564434506</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f t="shared" si="2"/>
         <v>35040000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+    <row r="18" spans="1:4">
+      <c r="A18" s="6">
         <f t="shared" si="1"/>
         <v>39598104.000078849</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <f t="shared" si="2"/>
         <v>37040000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+    <row r="19" spans="1:4">
+      <c r="A19" s="6">
         <f t="shared" si="1"/>
         <v>42014085.040079638</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <f t="shared" si="2"/>
         <v>39040000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+    <row r="20" spans="1:4">
+      <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>44454225.890480436</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <f t="shared" si="2"/>
         <v>41040000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+    <row r="21" spans="1:4">
+      <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>46918768.149385244</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <f t="shared" si="2"/>
         <v>43040000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+    <row r="22" spans="1:4">
+      <c r="A22" s="6">
         <f t="shared" si="1"/>
         <v>49407955.8308791</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <f t="shared" si="2"/>
         <v>45040000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+    <row r="23" spans="1:4">
+      <c r="A23" s="6">
         <f t="shared" si="1"/>
         <v>51922035.389187895</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <f t="shared" si="2"/>
         <v>47040000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+    <row r="24" spans="1:4">
+      <c r="A24" s="6">
         <f t="shared" si="1"/>
         <v>54461255.743079774</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>2</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <f>(C23+F$2)*D24</f>
         <v>51001600</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+    <row r="25" spans="1:4">
+      <c r="A25" s="6">
         <f t="shared" si="1"/>
         <v>57025868.30051057</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <f>C24+F$2</f>
         <v>53001600</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+    <row r="26" spans="1:4">
+      <c r="A26" s="6">
         <f t="shared" si="1"/>
         <v>59616126.98351568</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <f t="shared" ref="C26:C35" si="3">C25+F$2</f>
         <v>55001600</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+    <row r="27" spans="1:4">
+      <c r="A27" s="6">
         <f t="shared" si="1"/>
         <v>62232288.253350839</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <f t="shared" si="3"/>
         <v>57001600</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+    <row r="28" spans="1:4">
+      <c r="A28" s="6">
         <f t="shared" si="1"/>
         <v>64874611.135884345</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <f t="shared" si="3"/>
         <v>59001600</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+    <row r="29" spans="1:4">
+      <c r="A29" s="6">
         <f t="shared" si="1"/>
         <v>67543357.247243196</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <f t="shared" si="3"/>
         <v>61001600</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+    <row r="30" spans="1:4">
+      <c r="A30" s="6">
         <f t="shared" si="1"/>
         <v>70238790.819715634</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <f t="shared" si="3"/>
         <v>63001600</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
+    <row r="31" spans="1:4">
+      <c r="A31" s="6">
         <f t="shared" si="1"/>
         <v>72961178.727912784</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <f t="shared" si="3"/>
         <v>65001600</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
+    <row r="32" spans="1:4">
+      <c r="A32" s="6">
         <f t="shared" si="1"/>
         <v>75710790.515191913</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <f t="shared" si="3"/>
         <v>67001600</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+    <row r="33" spans="1:4">
+      <c r="A33" s="6">
         <f t="shared" si="1"/>
         <v>78487898.420343831</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <f t="shared" si="3"/>
         <v>69001600</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
+    <row r="34" spans="1:4">
+      <c r="A34" s="6">
         <f t="shared" si="1"/>
         <v>81292777.404547274</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <f t="shared" si="3"/>
         <v>71001600</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
+    <row r="35" spans="1:4">
+      <c r="A35" s="6">
         <f t="shared" si="1"/>
         <v>84125705.178592741</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <f t="shared" si="3"/>
         <v>73001600</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
+    <row r="36" spans="1:4">
+      <c r="A36" s="6">
         <f t="shared" si="1"/>
         <v>86986962.230378672</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>3</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <f>(C35+F$2)*D36</f>
         <v>78001664</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
+    <row r="37" spans="1:4">
+      <c r="A37" s="6">
         <f t="shared" si="1"/>
         <v>89876831.852682456</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <f>C36+F$2</f>
         <v>80001664</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
+    <row r="38" spans="1:4">
+      <c r="A38" s="6">
         <f t="shared" si="1"/>
         <v>92795600.171209276</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <f t="shared" ref="C38:C47" si="4">C37+F$2</f>
         <v>82001664</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
+    <row r="39" spans="1:4">
+      <c r="A39" s="6">
         <f t="shared" si="1"/>
         <v>95743556.172921374</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <f t="shared" si="4"/>
         <v>84001664</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
+    <row r="40" spans="1:4">
+      <c r="A40" s="6">
         <f t="shared" si="1"/>
         <v>98720991.734650582</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <f t="shared" si="4"/>
         <v>86001664</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
+    <row r="41" spans="1:4">
+      <c r="A41" s="6">
         <f t="shared" si="1"/>
         <v>101728201.65199709</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <f t="shared" si="4"/>
         <v>88001664</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
+    <row r="42" spans="1:4">
+      <c r="A42" s="6">
         <f t="shared" si="1"/>
         <v>104765483.66851707</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="6">
         <f t="shared" si="4"/>
         <v>90001664</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
+    <row r="43" spans="1:4">
+      <c r="A43" s="6">
         <f t="shared" si="1"/>
         <v>107833138.50520223</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="6">
         <f t="shared" si="4"/>
         <v>92001664</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
+    <row r="44" spans="1:4">
+      <c r="A44" s="6">
         <f t="shared" si="1"/>
         <v>110931469.89025426</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="6">
         <f t="shared" si="4"/>
         <v>94001664</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
+    <row r="45" spans="1:4">
+      <c r="A45" s="6">
         <f t="shared" si="1"/>
         <v>114060784.58915681</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <f t="shared" si="4"/>
         <v>96001664</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
+    <row r="46" spans="1:4">
+      <c r="A46" s="6">
         <f t="shared" si="1"/>
         <v>117221392.43504837</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <f t="shared" si="4"/>
         <v>98001664</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
+    <row r="47" spans="1:4">
+      <c r="A47" s="6">
         <f t="shared" si="1"/>
         <v>120413606.35939886</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <f t="shared" si="4"/>
         <v>100001664</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
+    <row r="48" spans="1:4">
+      <c r="A48" s="6">
         <f t="shared" si="1"/>
         <v>123637742.42299284</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <v>4</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="6">
         <f>(C47+F$2)*D48</f>
         <v>106081730.56</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
+    <row r="49" spans="1:4">
+      <c r="A49" s="6">
         <f t="shared" si="1"/>
         <v>126894119.84722278</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <f>C48+F$2</f>
         <v>108081730.56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
+    <row r="50" spans="1:4">
+      <c r="A50" s="6">
         <f t="shared" si="1"/>
         <v>130183061.04569501</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <f t="shared" ref="C50:C59" si="5">C49+F$2</f>
         <v>110081730.56</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
+    <row r="51" spans="1:4">
+      <c r="A51" s="6">
         <f t="shared" si="1"/>
         <v>133504891.65615197</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <f t="shared" si="5"/>
         <v>112081730.56</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="7">
+    <row r="52" spans="1:4">
+      <c r="A52" s="6">
         <f t="shared" si="1"/>
         <v>136859940.57271346</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="6">
         <f t="shared" si="5"/>
         <v>114081730.56</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
+    <row r="53" spans="1:4">
+      <c r="A53" s="6">
         <f t="shared" si="1"/>
         <v>140248539.97844061</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="6">
         <f t="shared" si="5"/>
         <v>116081730.56</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="7">
+    <row r="54" spans="1:4">
+      <c r="A54" s="6">
         <f t="shared" si="1"/>
         <v>143671025.37822503</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="6">
         <f t="shared" si="5"/>
         <v>118081730.56</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="7">
+    <row r="55" spans="1:4">
+      <c r="A55" s="6">
         <f t="shared" si="1"/>
         <v>147127735.63200727</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="6">
         <f t="shared" si="5"/>
         <v>120081730.56</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="7">
+    <row r="56" spans="1:4">
+      <c r="A56" s="6">
         <f t="shared" si="1"/>
         <v>150619012.98832735</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="6">
         <f t="shared" si="5"/>
         <v>122081730.56</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="7">
+    <row r="57" spans="1:4">
+      <c r="A57" s="6">
         <f t="shared" si="1"/>
         <v>154145203.11821064</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="6">
         <f t="shared" si="5"/>
         <v>124081730.56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="7">
+    <row r="58" spans="1:4">
+      <c r="A58" s="6">
         <f t="shared" si="1"/>
         <v>157706655.14939275</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="6">
         <f t="shared" si="5"/>
         <v>126081730.56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
+    <row r="59" spans="1:4">
+      <c r="A59" s="6">
         <f t="shared" si="1"/>
         <v>161303721.7008867</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="6">
         <f t="shared" si="5"/>
         <v>128081730.56</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="7">
+    <row r="60" spans="1:4">
+      <c r="A60" s="6">
         <f t="shared" si="1"/>
         <v>164936758.91789556</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <v>5</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="6">
         <f>(C59+F$2)*D60</f>
         <v>135284999.78240001</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
+    <row r="61" spans="1:4">
+      <c r="A61" s="6">
         <f t="shared" si="1"/>
         <v>168606126.50707451</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="6">
         <f>C60+F$2</f>
         <v>137284999.78240001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="7">
+    <row r="62" spans="1:4">
+      <c r="A62" s="6">
         <f t="shared" si="1"/>
         <v>172312187.77214524</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="6">
         <f t="shared" ref="C62:C71" si="6">C61+F$2</f>
         <v>139284999.78240001</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="7">
+    <row r="63" spans="1:4">
+      <c r="A63" s="6">
         <f t="shared" si="1"/>
         <v>176055309.6498667</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <f t="shared" si="6"/>
         <v>141284999.78240001</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="7">
+    <row r="64" spans="1:4">
+      <c r="A64" s="6">
         <f t="shared" si="1"/>
         <v>179835862.74636537</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="6">
         <f t="shared" si="6"/>
         <v>143284999.78240001</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="7">
+    <row r="65" spans="1:4">
+      <c r="A65" s="6">
         <f t="shared" si="1"/>
         <v>183654221.37382904</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <f t="shared" si="6"/>
         <v>145284999.78240001</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="7">
+    <row r="66" spans="1:4">
+      <c r="A66" s="6">
         <f t="shared" si="1"/>
         <v>187510763.58756733</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="6">
         <f t="shared" si="6"/>
         <v>147284999.78240001</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="7">
+    <row r="67" spans="1:4">
+      <c r="A67" s="6">
         <f t="shared" si="1"/>
         <v>191405871.223443</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="6">
         <f t="shared" si="6"/>
         <v>149284999.78240001</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="7">
+    <row r="68" spans="1:4">
+      <c r="A68" s="6">
         <f t="shared" si="1"/>
         <v>195339929.93567744</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="6">
         <f t="shared" si="6"/>
         <v>151284999.78240001</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="7">
+    <row r="69" spans="1:4">
+      <c r="A69" s="6">
         <f t="shared" ref="A69:A132" si="7">(A68+F$2)*G$2</f>
         <v>199313329.23503423</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="6">
         <f t="shared" si="6"/>
         <v>153284999.78240001</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="7">
+    <row r="70" spans="1:4">
+      <c r="A70" s="6">
         <f t="shared" si="7"/>
         <v>203326462.52738458</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="6">
         <f t="shared" si="6"/>
         <v>155284999.78240001</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="7">
+    <row r="71" spans="1:4">
+      <c r="A71" s="6">
         <f t="shared" si="7"/>
         <v>207379727.15265843</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="6">
         <f t="shared" si="6"/>
         <v>157284999.78240001</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="7">
+    <row r="72" spans="1:4">
+      <c r="A72" s="6">
         <f t="shared" si="7"/>
         <v>211473524.42418501</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="6">
         <v>6</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="6">
         <f>(C71+F$2)*D72</f>
         <v>165656399.77369601</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="7">
+    <row r="73" spans="1:4">
+      <c r="A73" s="6">
         <f t="shared" si="7"/>
         <v>215608259.66842687</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <f>C72+F$2</f>
         <v>167656399.77369601</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="7">
+    <row r="74" spans="1:4">
+      <c r="A74" s="6">
         <f t="shared" si="7"/>
         <v>219784342.26511115</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="6">
         <f t="shared" ref="C74:C83" si="8">C73+F$2</f>
         <v>169656399.77369601</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="7">
+    <row r="75" spans="1:4">
+      <c r="A75" s="6">
         <f t="shared" si="7"/>
         <v>224002185.68776226</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="6">
         <f t="shared" si="8"/>
         <v>171656399.77369601</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="7">
+    <row r="76" spans="1:4">
+      <c r="A76" s="6">
         <f t="shared" si="7"/>
         <v>228262207.54463989</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="6">
         <f t="shared" si="8"/>
         <v>173656399.77369601</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="7">
+    <row r="77" spans="1:4">
+      <c r="A77" s="6">
         <f t="shared" si="7"/>
         <v>232564829.62008628</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="6">
         <f t="shared" si="8"/>
         <v>175656399.77369601</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="7">
+    <row r="78" spans="1:4">
+      <c r="A78" s="6">
         <f t="shared" si="7"/>
         <v>236910477.91628715</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="6">
         <f t="shared" si="8"/>
         <v>177656399.77369601</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="7">
+    <row r="79" spans="1:4">
+      <c r="A79" s="6">
         <f t="shared" si="7"/>
         <v>241299582.69545004</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="6">
         <f t="shared" si="8"/>
         <v>179656399.77369601</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="7">
+    <row r="80" spans="1:4">
+      <c r="A80" s="6">
         <f t="shared" si="7"/>
         <v>245732578.52240455</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="6">
         <f t="shared" si="8"/>
         <v>181656399.77369601</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="7">
+    <row r="81" spans="1:4">
+      <c r="A81" s="6">
         <f t="shared" si="7"/>
         <v>250209904.3076286</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="6">
         <f t="shared" si="8"/>
         <v>183656399.77369601</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="7">
+    <row r="82" spans="1:4">
+      <c r="A82" s="6">
         <f t="shared" si="7"/>
         <v>254732003.35070488</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="6">
         <f t="shared" si="8"/>
         <v>185656399.77369601</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="7">
+    <row r="83" spans="1:4">
+      <c r="A83" s="6">
         <f t="shared" si="7"/>
         <v>259299323.38421193</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="6">
         <f t="shared" si="8"/>
         <v>187656399.77369601</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="7">
+    <row r="84" spans="1:4">
+      <c r="A84" s="6">
         <f t="shared" si="7"/>
         <v>263912316.61805406</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84" s="6">
         <v>7</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="6">
         <f>(C83+F$2)*D84</f>
         <v>197242655.76464385</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="7">
+    <row r="85" spans="1:4">
+      <c r="A85" s="6">
         <f t="shared" si="7"/>
         <v>268571439.78423458</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="6">
         <f>C84+F$2</f>
         <v>199242655.76464385</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="7">
+    <row r="86" spans="1:4">
+      <c r="A86" s="6">
         <f t="shared" si="7"/>
         <v>273277154.18207693</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="6">
         <f t="shared" ref="C86:C95" si="9">C85+F$2</f>
         <v>201242655.76464385</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="7">
+    <row r="87" spans="1:4">
+      <c r="A87" s="6">
         <f t="shared" si="7"/>
         <v>278029925.7238977</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="6">
         <f t="shared" si="9"/>
         <v>203242655.76464385</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="7">
+    <row r="88" spans="1:4">
+      <c r="A88" s="6">
         <f t="shared" si="7"/>
         <v>282830224.98113668</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C88" s="6">
         <f t="shared" si="9"/>
         <v>205242655.76464385</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="7">
+    <row r="89" spans="1:4">
+      <c r="A89" s="6">
         <f t="shared" si="7"/>
         <v>287678527.23094803</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="6">
         <f t="shared" si="9"/>
         <v>207242655.76464385</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="7">
+    <row r="90" spans="1:4">
+      <c r="A90" s="6">
         <f t="shared" si="7"/>
         <v>292575312.50325751</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="6">
         <f t="shared" si="9"/>
         <v>209242655.76464385</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="7">
+    <row r="91" spans="1:4">
+      <c r="A91" s="6">
         <f t="shared" si="7"/>
         <v>297521065.62829012</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="6">
         <f t="shared" si="9"/>
         <v>211242655.76464385</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="7">
+    <row r="92" spans="1:4">
+      <c r="A92" s="6">
         <f t="shared" si="7"/>
         <v>302516276.28457302</v>
       </c>
-      <c r="C92" s="7">
+      <c r="C92" s="6">
         <f t="shared" si="9"/>
         <v>213242655.76464385</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="7">
+    <row r="93" spans="1:4">
+      <c r="A93" s="6">
         <f t="shared" si="7"/>
         <v>307561439.04741877</v>
       </c>
-      <c r="C93" s="7">
+      <c r="C93" s="6">
         <f t="shared" si="9"/>
         <v>215242655.76464385</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="7">
+    <row r="94" spans="1:4">
+      <c r="A94" s="6">
         <f t="shared" si="7"/>
         <v>312657053.43789297</v>
       </c>
-      <c r="C94" s="7">
+      <c r="C94" s="6">
         <f t="shared" si="9"/>
         <v>217242655.76464385</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="7">
+    <row r="95" spans="1:4">
+      <c r="A95" s="6">
         <f t="shared" si="7"/>
         <v>317803623.97227192</v>
       </c>
-      <c r="C95" s="7">
+      <c r="C95" s="6">
         <f t="shared" si="9"/>
         <v>219242655.76464385</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="7">
+    <row r="96" spans="1:4">
+      <c r="A96" s="6">
         <f t="shared" si="7"/>
         <v>323001660.21199465</v>
       </c>
-      <c r="B96" s="7">
+      <c r="B96" s="6">
         <v>8</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="6">
         <f>(C95+F$2)*D96</f>
         <v>230092361.9952296</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="7">
+    <row r="97" spans="1:4">
+      <c r="A97" s="6">
         <f t="shared" si="7"/>
         <v>328251676.81411457</v>
       </c>
-      <c r="C97" s="7">
+      <c r="C97" s="6">
         <f>C96+F$2</f>
         <v>232092361.9952296</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="7">
+    <row r="98" spans="1:4">
+      <c r="A98" s="6">
         <f t="shared" si="7"/>
         <v>333554193.58225572</v>
       </c>
-      <c r="C98" s="7">
+      <c r="C98" s="6">
         <f t="shared" ref="C98:C107" si="10">C97+F$2</f>
         <v>234092361.9952296</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="7">
+    <row r="99" spans="1:4">
+      <c r="A99" s="6">
         <f t="shared" si="7"/>
         <v>338909735.51807827</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="6">
         <f t="shared" si="10"/>
         <v>236092361.9952296</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="7">
+    <row r="100" spans="1:4">
+      <c r="A100" s="6">
         <f t="shared" si="7"/>
         <v>344318832.87325907</v>
       </c>
-      <c r="C100" s="7">
+      <c r="C100" s="6">
         <f t="shared" si="10"/>
         <v>238092361.9952296</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="7">
+    <row r="101" spans="1:4">
+      <c r="A101" s="6">
         <f t="shared" si="7"/>
         <v>349782021.20199168</v>
       </c>
-      <c r="C101" s="7">
+      <c r="C101" s="6">
         <f t="shared" si="10"/>
         <v>240092361.9952296</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="7">
+    <row r="102" spans="1:4">
+      <c r="A102" s="6">
         <f t="shared" si="7"/>
         <v>355299841.4140116</v>
       </c>
-      <c r="C102" s="7">
+      <c r="C102" s="6">
         <f t="shared" si="10"/>
         <v>242092361.9952296</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="7">
+    <row r="103" spans="1:4">
+      <c r="A103" s="6">
         <f t="shared" si="7"/>
         <v>360872839.8281517</v>
       </c>
-      <c r="C103" s="7">
+      <c r="C103" s="6">
         <f t="shared" si="10"/>
         <v>244092361.9952296</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="7">
+    <row r="104" spans="1:4">
+      <c r="A104" s="6">
         <f t="shared" si="7"/>
         <v>366501568.22643322</v>
       </c>
-      <c r="C104" s="7">
+      <c r="C104" s="6">
         <f t="shared" si="10"/>
         <v>246092361.9952296</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="7">
+    <row r="105" spans="1:4">
+      <c r="A105" s="6">
         <f t="shared" si="7"/>
         <v>372186583.90869755</v>
       </c>
-      <c r="C105" s="7">
+      <c r="C105" s="6">
         <f t="shared" si="10"/>
         <v>248092361.9952296</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="7">
+    <row r="106" spans="1:4">
+      <c r="A106" s="6">
         <f t="shared" si="7"/>
         <v>377928449.7477845</v>
       </c>
-      <c r="C106" s="7">
+      <c r="C106" s="6">
         <f t="shared" si="10"/>
         <v>250092361.9952296</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="7">
+    <row r="107" spans="1:4">
+      <c r="A107" s="6">
         <f t="shared" si="7"/>
         <v>383727734.24526232</v>
       </c>
-      <c r="C107" s="7">
+      <c r="C107" s="6">
         <f t="shared" si="10"/>
         <v>252092361.9952296</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="7">
+    <row r="108" spans="1:4">
+      <c r="A108" s="6">
         <f t="shared" si="7"/>
         <v>389585011.58771497</v>
       </c>
-      <c r="B108" s="7">
+      <c r="B108" s="6">
         <v>9</v>
       </c>
-      <c r="C108" s="7">
+      <c r="C108" s="6">
         <f>(C107+F$2)*D108</f>
         <v>264256056.4750388</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="7">
+    <row r="109" spans="1:4">
+      <c r="A109" s="6">
         <f t="shared" si="7"/>
         <v>395500861.70359212</v>
       </c>
-      <c r="C109" s="7">
+      <c r="C109" s="6">
         <f>C108+F$2</f>
         <v>266256056.4750388</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="7">
+    <row r="110" spans="1:4">
+      <c r="A110" s="6">
         <f t="shared" si="7"/>
         <v>401475870.32062805</v>
       </c>
-      <c r="C110" s="7">
+      <c r="C110" s="6">
         <f t="shared" ref="C110:C119" si="11">C109+F$2</f>
         <v>268256056.4750388</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="7">
+    <row r="111" spans="1:4">
+      <c r="A111" s="6">
         <f t="shared" si="7"/>
         <v>407510629.02383435</v>
       </c>
-      <c r="C111" s="7">
+      <c r="C111" s="6">
         <f t="shared" si="11"/>
         <v>270256056.47503877</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="7">
+    <row r="112" spans="1:4">
+      <c r="A112" s="6">
         <f t="shared" si="7"/>
         <v>413605735.31407267</v>
       </c>
-      <c r="C112" s="7">
+      <c r="C112" s="6">
         <f t="shared" si="11"/>
         <v>272256056.47503877</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="7">
+    <row r="113" spans="1:4">
+      <c r="A113" s="6">
         <f t="shared" si="7"/>
         <v>419761792.66721338</v>
       </c>
-      <c r="C113" s="7">
+      <c r="C113" s="6">
         <f t="shared" si="11"/>
         <v>274256056.47503877</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="7">
+    <row r="114" spans="1:4">
+      <c r="A114" s="6">
         <f t="shared" si="7"/>
         <v>425979410.59388554</v>
       </c>
-      <c r="C114" s="7">
+      <c r="C114" s="6">
         <f t="shared" si="11"/>
         <v>276256056.47503877</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="7">
+    <row r="115" spans="1:4">
+      <c r="A115" s="6">
         <f t="shared" si="7"/>
         <v>432259204.69982439</v>
       </c>
-      <c r="C115" s="7">
+      <c r="C115" s="6">
         <f t="shared" si="11"/>
         <v>278256056.47503877</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="7">
+    <row r="116" spans="1:4">
+      <c r="A116" s="6">
         <f t="shared" si="7"/>
         <v>438601796.74682266</v>
       </c>
-      <c r="C116" s="7">
+      <c r="C116" s="6">
         <f t="shared" si="11"/>
         <v>280256056.47503877</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" s="7">
+    <row r="117" spans="1:4">
+      <c r="A117" s="6">
         <f t="shared" si="7"/>
         <v>445007814.71429086</v>
       </c>
-      <c r="C117" s="7">
+      <c r="C117" s="6">
         <f t="shared" si="11"/>
         <v>282256056.47503877</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="7">
+    <row r="118" spans="1:4">
+      <c r="A118" s="6">
         <f t="shared" si="7"/>
         <v>451477892.86143374</v>
       </c>
-      <c r="C118" s="7">
+      <c r="C118" s="6">
         <f t="shared" si="11"/>
         <v>284256056.47503877</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" s="7">
+    <row r="119" spans="1:4">
+      <c r="A119" s="6">
         <f t="shared" si="7"/>
         <v>458012671.79004806</v>
       </c>
-      <c r="C119" s="7">
+      <c r="C119" s="6">
         <f t="shared" si="11"/>
         <v>286256056.47503877</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="7">
+    <row r="120" spans="1:4">
+      <c r="A120" s="6">
         <f t="shared" si="7"/>
         <v>464612798.50794852</v>
       </c>
-      <c r="B120" s="7">
+      <c r="B120" s="6">
         <v>10</v>
       </c>
-      <c r="C120" s="7">
+      <c r="C120" s="6">
         <f>(C119+F$2)*D120</f>
         <v>299786298.73404032</v>
       </c>
-      <c r="D120" s="3">
+      <c r="D120" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" s="7">
+    <row r="121" spans="1:4">
+      <c r="A121" s="6">
         <f t="shared" si="7"/>
         <v>471278926.49302799</v>
       </c>
-      <c r="C121" s="7">
+      <c r="C121" s="6">
         <f>C120+F$2</f>
         <v>301786298.73404032</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" s="7">
+    <row r="122" spans="1:4">
+      <c r="A122" s="6">
         <f t="shared" si="7"/>
         <v>478011715.75795829</v>
       </c>
-      <c r="C122" s="7">
+      <c r="C122" s="6">
         <f t="shared" ref="C122:C131" si="12">C121+F$2</f>
         <v>303786298.73404032</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="7">
+    <row r="123" spans="1:4">
+      <c r="A123" s="6">
         <f t="shared" si="7"/>
         <v>484811832.91553789</v>
       </c>
-      <c r="C123" s="7">
+      <c r="C123" s="6">
         <f t="shared" si="12"/>
         <v>305786298.73404032</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="7">
+    <row r="124" spans="1:4">
+      <c r="A124" s="6">
         <f t="shared" si="7"/>
         <v>491679951.24469328</v>
       </c>
-      <c r="C124" s="7">
+      <c r="C124" s="6">
         <f t="shared" si="12"/>
         <v>307786298.73404032</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="7">
+    <row r="125" spans="1:4">
+      <c r="A125" s="6">
         <f t="shared" si="7"/>
         <v>498616750.75714022</v>
       </c>
-      <c r="C125" s="7">
+      <c r="C125" s="6">
         <f t="shared" si="12"/>
         <v>309786298.73404032</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="7">
+    <row r="126" spans="1:4">
+      <c r="A126" s="6">
         <f t="shared" si="7"/>
         <v>505622918.26471162</v>
       </c>
-      <c r="C126" s="7">
+      <c r="C126" s="6">
         <f t="shared" si="12"/>
         <v>311786298.73404032</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="7">
+    <row r="127" spans="1:4">
+      <c r="A127" s="6">
         <f t="shared" si="7"/>
         <v>512699147.44735873</v>
       </c>
-      <c r="C127" s="7">
+      <c r="C127" s="6">
         <f t="shared" si="12"/>
         <v>313786298.73404032</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" s="7">
+    <row r="128" spans="1:4">
+      <c r="A128" s="6">
         <f t="shared" si="7"/>
         <v>519846138.92183232</v>
       </c>
-      <c r="C128" s="7">
+      <c r="C128" s="6">
         <f t="shared" si="12"/>
         <v>315786298.73404032</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="7">
+    <row r="129" spans="1:4">
+      <c r="A129" s="6">
         <f t="shared" si="7"/>
         <v>527064600.31105065</v>
       </c>
-      <c r="C129" s="7">
+      <c r="C129" s="6">
         <f t="shared" si="12"/>
         <v>317786298.73404032</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" s="7">
+    <row r="130" spans="1:4">
+      <c r="A130" s="6">
         <f t="shared" si="7"/>
         <v>534355246.31416118</v>
       </c>
-      <c r="C130" s="7">
+      <c r="C130" s="6">
         <f t="shared" si="12"/>
         <v>319786298.73404032</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="7">
+    <row r="131" spans="1:4">
+      <c r="A131" s="6">
         <f t="shared" si="7"/>
         <v>541718798.77730274</v>
       </c>
-      <c r="C131" s="7">
+      <c r="C131" s="6">
         <f t="shared" si="12"/>
         <v>321786298.73404032</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" s="7">
+    <row r="132" spans="1:4">
+      <c r="A132" s="6">
         <f t="shared" si="7"/>
         <v>549155986.7650758</v>
       </c>
-      <c r="B132" s="7">
+      <c r="B132" s="6">
         <v>11</v>
       </c>
-      <c r="C132" s="7">
+      <c r="C132" s="6">
         <f>(C131+F$2)*D132</f>
         <v>336737750.68340194</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D132" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" s="7">
-        <f t="shared" ref="A133:A170" si="13">(A132+F$2)*G$2</f>
+    <row r="133" spans="1:4">
+      <c r="A133" s="6">
+        <f t="shared" ref="A133:A168" si="13">(A132+F$2)*G$2</f>
         <v>556667546.63272655</v>
       </c>
-      <c r="C133" s="7">
+      <c r="C133" s="6">
         <f>C132+F$2</f>
         <v>338737750.68340194</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" s="7">
+    <row r="134" spans="1:4">
+      <c r="A134" s="6">
         <f t="shared" si="13"/>
         <v>564254222.09905386</v>
       </c>
-      <c r="C134" s="7">
+      <c r="C134" s="6">
         <f t="shared" ref="C134:C143" si="14">C133+F$2</f>
         <v>340737750.68340194</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" s="7">
+    <row r="135" spans="1:4">
+      <c r="A135" s="6">
         <f t="shared" si="13"/>
         <v>571916764.3200444</v>
       </c>
-      <c r="C135" s="7">
+      <c r="C135" s="6">
         <f t="shared" si="14"/>
         <v>342737750.68340194</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" s="7">
+    <row r="136" spans="1:4">
+      <c r="A136" s="6">
         <f t="shared" si="13"/>
         <v>579655931.9632448</v>
       </c>
-      <c r="C136" s="7">
+      <c r="C136" s="6">
         <f t="shared" si="14"/>
         <v>344737750.68340194</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" s="7">
+    <row r="137" spans="1:4">
+      <c r="A137" s="6">
         <f t="shared" si="13"/>
         <v>587472491.28287721</v>
       </c>
-      <c r="C137" s="7">
+      <c r="C137" s="6">
         <f t="shared" si="14"/>
         <v>346737750.68340194</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" s="7">
+    <row r="138" spans="1:4">
+      <c r="A138" s="6">
         <f t="shared" si="13"/>
         <v>595367216.19570601</v>
       </c>
-      <c r="C138" s="7">
+      <c r="C138" s="6">
         <f t="shared" si="14"/>
         <v>348737750.68340194</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" s="7">
+    <row r="139" spans="1:4">
+      <c r="A139" s="6">
         <f t="shared" si="13"/>
         <v>603340888.35766304</v>
       </c>
-      <c r="C139" s="7">
+      <c r="C139" s="6">
         <f t="shared" si="14"/>
         <v>350737750.68340194</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" s="7">
+    <row r="140" spans="1:4">
+      <c r="A140" s="6">
         <f t="shared" si="13"/>
         <v>611394297.24123967</v>
       </c>
-      <c r="C140" s="7">
+      <c r="C140" s="6">
         <f t="shared" si="14"/>
         <v>352737750.68340194</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" s="7">
+    <row r="141" spans="1:4">
+      <c r="A141" s="6">
         <f t="shared" si="13"/>
         <v>619528240.21365201</v>
       </c>
-      <c r="C141" s="7">
+      <c r="C141" s="6">
         <f t="shared" si="14"/>
         <v>354737750.68340194</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" s="7">
+    <row r="142" spans="1:4">
+      <c r="A142" s="6">
         <f t="shared" si="13"/>
         <v>627743522.61578858</v>
       </c>
-      <c r="C142" s="7">
+      <c r="C142" s="6">
         <f t="shared" si="14"/>
         <v>356737750.68340194</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" s="7">
+    <row r="143" spans="1:4">
+      <c r="A143" s="6">
         <f t="shared" si="13"/>
         <v>636040957.84194648</v>
       </c>
-      <c r="C143" s="7">
+      <c r="C143" s="6">
         <f t="shared" si="14"/>
         <v>358737750.68340194</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" s="7">
+    <row r="144" spans="1:4">
+      <c r="A144" s="6">
         <f t="shared" si="13"/>
         <v>644421367.42036593</v>
       </c>
-      <c r="B144" s="7">
+      <c r="B144" s="6">
         <v>12</v>
       </c>
-      <c r="C144" s="7">
+      <c r="C144" s="6">
         <f>(C143+F$2)*D144</f>
         <v>375167260.710738</v>
       </c>
-      <c r="D144" s="3">
+      <c r="D144" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" s="7">
+    <row r="145" spans="1:4">
+      <c r="A145" s="6">
         <f t="shared" si="13"/>
         <v>652885581.09456956</v>
       </c>
-      <c r="C145" s="7">
+      <c r="C145" s="6">
         <f>C144+F$2</f>
         <v>377167260.710738</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" s="7">
+    <row r="146" spans="1:4">
+      <c r="A146" s="6">
         <f t="shared" si="13"/>
         <v>661434436.90551531</v>
       </c>
-      <c r="C146" s="7">
+      <c r="C146" s="6">
         <f t="shared" ref="C146:C155" si="15">C145+F$2</f>
         <v>379167260.710738</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="7">
+    <row r="147" spans="1:4">
+      <c r="A147" s="6">
         <f t="shared" si="13"/>
         <v>670068781.27457047</v>
       </c>
-      <c r="C147" s="7">
+      <c r="C147" s="6">
         <f t="shared" si="15"/>
         <v>381167260.710738</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="7">
+    <row r="148" spans="1:4">
+      <c r="A148" s="6">
         <f t="shared" si="13"/>
         <v>678789469.08731616</v>
       </c>
-      <c r="C148" s="7">
+      <c r="C148" s="6">
         <f t="shared" si="15"/>
         <v>383167260.710738</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" s="7">
+    <row r="149" spans="1:4">
+      <c r="A149" s="6">
         <f t="shared" si="13"/>
         <v>687597363.7781893</v>
       </c>
-      <c r="C149" s="7">
+      <c r="C149" s="6">
         <f t="shared" si="15"/>
         <v>385167260.710738</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" s="7">
+    <row r="150" spans="1:4">
+      <c r="A150" s="6">
         <f t="shared" si="13"/>
         <v>696493337.41597116</v>
       </c>
-      <c r="C150" s="7">
+      <c r="C150" s="6">
         <f t="shared" si="15"/>
         <v>387167260.710738</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" s="7">
+    <row r="151" spans="1:4">
+      <c r="A151" s="6">
         <f t="shared" si="13"/>
         <v>705478270.79013085</v>
       </c>
-      <c r="C151" s="7">
+      <c r="C151" s="6">
         <f t="shared" si="15"/>
         <v>389167260.710738</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" s="7">
+    <row r="152" spans="1:4">
+      <c r="A152" s="6">
         <f t="shared" si="13"/>
         <v>714553053.49803221</v>
       </c>
-      <c r="C152" s="7">
+      <c r="C152" s="6">
         <f t="shared" si="15"/>
         <v>391167260.710738</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="7">
+    <row r="153" spans="1:4">
+      <c r="A153" s="6">
         <f t="shared" si="13"/>
         <v>723718584.03301251</v>
       </c>
-      <c r="C153" s="7">
+      <c r="C153" s="6">
         <f t="shared" si="15"/>
         <v>393167260.710738</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" s="7">
+    <row r="154" spans="1:4">
+      <c r="A154" s="6">
         <f t="shared" si="13"/>
         <v>732975769.87334263</v>
       </c>
-      <c r="C154" s="7">
+      <c r="C154" s="6">
         <f t="shared" si="15"/>
         <v>395167260.710738</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" s="7">
+    <row r="155" spans="1:4">
+      <c r="A155" s="6">
         <f t="shared" si="13"/>
         <v>742325527.57207608</v>
       </c>
-      <c r="C155" s="7">
+      <c r="C155" s="6">
         <f t="shared" si="15"/>
         <v>397167260.710738</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" s="7">
+    <row r="156" spans="1:4">
+      <c r="A156" s="6">
         <f t="shared" si="13"/>
         <v>751768782.8477968</v>
       </c>
-      <c r="B156" s="7">
+      <c r="B156" s="6">
         <v>13</v>
       </c>
-      <c r="C156" s="7">
+      <c r="C156" s="6">
         <f>(C155+F$2)*D156</f>
         <v>415133951.13916755</v>
       </c>
-      <c r="D156" s="3">
+      <c r="D156" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" s="7">
+    <row r="157" spans="1:4">
+      <c r="A157" s="6">
         <f t="shared" si="13"/>
         <v>761306470.67627478</v>
       </c>
-      <c r="C157" s="7">
+      <c r="C157" s="6">
         <f>C156+F$2</f>
         <v>417133951.13916755</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" s="7">
+    <row r="158" spans="1:4">
+      <c r="A158" s="6">
         <f t="shared" si="13"/>
         <v>770939535.38303757</v>
       </c>
-      <c r="C158" s="7">
+      <c r="C158" s="6">
         <f t="shared" ref="C158:C167" si="16">C157+F$2</f>
         <v>419133951.13916755</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" s="7">
+    <row r="159" spans="1:4">
+      <c r="A159" s="6">
         <f t="shared" si="13"/>
         <v>780668930.7368679</v>
       </c>
-      <c r="C159" s="7">
+      <c r="C159" s="6">
         <f t="shared" si="16"/>
         <v>421133951.13916755</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" s="7">
+    <row r="160" spans="1:4">
+      <c r="A160" s="6">
         <f t="shared" si="13"/>
         <v>790495620.04423654</v>
       </c>
-      <c r="C160" s="7">
+      <c r="C160" s="6">
         <f t="shared" si="16"/>
         <v>423133951.13916755</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" s="7">
+    <row r="161" spans="1:4">
+      <c r="A161" s="6">
         <f t="shared" si="13"/>
         <v>800420576.24467885</v>
       </c>
-      <c r="C161" s="7">
+      <c r="C161" s="6">
         <f t="shared" si="16"/>
         <v>425133951.13916755</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" s="7">
+    <row r="162" spans="1:4">
+      <c r="A162" s="6">
         <f t="shared" si="13"/>
         <v>810444782.00712562</v>
       </c>
-      <c r="C162" s="7">
+      <c r="C162" s="6">
         <f t="shared" si="16"/>
         <v>427133951.13916755</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" s="7">
+    <row r="163" spans="1:4">
+      <c r="A163" s="6">
         <f t="shared" si="13"/>
         <v>820569229.82719684</v>
       </c>
-      <c r="C163" s="7">
+      <c r="C163" s="6">
         <f t="shared" si="16"/>
         <v>429133951.13916755</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A164" s="7">
+    <row r="164" spans="1:4">
+      <c r="A164" s="6">
         <f t="shared" si="13"/>
         <v>830794922.12546885</v>
       </c>
-      <c r="C164" s="7">
+      <c r="C164" s="6">
         <f t="shared" si="16"/>
         <v>431133951.13916755</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A165" s="7">
+    <row r="165" spans="1:4">
+      <c r="A165" s="6">
         <f t="shared" si="13"/>
         <v>841122871.34672356</v>
       </c>
-      <c r="C165" s="7">
+      <c r="C165" s="6">
         <f t="shared" si="16"/>
         <v>433133951.13916755</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" s="7">
+    <row r="166" spans="1:4">
+      <c r="A166" s="6">
         <f t="shared" si="13"/>
         <v>851554100.0601908</v>
       </c>
-      <c r="C166" s="7">
+      <c r="C166" s="6">
         <f t="shared" si="16"/>
         <v>435133951.13916755</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" s="7">
+    <row r="167" spans="1:4">
+      <c r="A167" s="6">
         <f t="shared" si="13"/>
         <v>862089641.06079268</v>
       </c>
-      <c r="C167" s="7">
+      <c r="C167" s="6">
         <f t="shared" si="16"/>
         <v>437133951.13916755</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" s="7">
+    <row r="168" spans="1:4">
+      <c r="A168" s="6">
         <f t="shared" si="13"/>
         <v>872730537.47140062</v>
       </c>
-      <c r="B168" s="7">
+      <c r="B168" s="6">
         <v>14</v>
       </c>
-      <c r="C168" s="7">
+      <c r="C168" s="6">
         <f>(C167+F$2)*D168</f>
         <v>456699309.18473428</v>
       </c>
-      <c r="D168" s="3">
+      <c r="D168" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" s="7">
+    <row r="169" spans="1:4">
+      <c r="A169" s="6">
         <f t="shared" ref="A169:A180" si="17">(A168+F$2)*G$2</f>
         <v>883477842.84611464</v>
       </c>
-      <c r="C169" s="7">
+      <c r="C169" s="6">
         <f>C168+F$2</f>
         <v>458699309.18473428</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" s="7">
+    <row r="170" spans="1:4">
+      <c r="A170" s="6">
         <f t="shared" si="17"/>
         <v>894332621.27457583</v>
       </c>
-      <c r="C170" s="7">
+      <c r="C170" s="6">
         <f t="shared" ref="C170:C179" si="18">C169+F$2</f>
         <v>460699309.18473428</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" s="7">
+    <row r="171" spans="1:4">
+      <c r="A171" s="6">
         <f t="shared" si="17"/>
         <v>905295947.48732162</v>
       </c>
-      <c r="C171" s="7">
+      <c r="C171" s="6">
         <f t="shared" si="18"/>
         <v>462699309.18473428</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" s="7">
+    <row r="172" spans="1:4">
+      <c r="A172" s="6">
         <f t="shared" si="17"/>
         <v>916368906.9621948</v>
       </c>
-      <c r="C172" s="7">
+      <c r="C172" s="6">
         <f t="shared" si="18"/>
         <v>464699309.18473428</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" s="7">
+    <row r="173" spans="1:4">
+      <c r="A173" s="6">
         <f t="shared" si="17"/>
         <v>927552596.03181672</v>
       </c>
-      <c r="C173" s="7">
+      <c r="C173" s="6">
         <f t="shared" si="18"/>
         <v>466699309.18473428</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" s="7">
+    <row r="174" spans="1:4">
+      <c r="A174" s="6">
         <f t="shared" si="17"/>
         <v>938848121.99213493</v>
       </c>
-      <c r="C174" s="7">
+      <c r="C174" s="6">
         <f t="shared" si="18"/>
         <v>468699309.18473428</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" s="7">
+    <row r="175" spans="1:4">
+      <c r="A175" s="6">
         <f t="shared" si="17"/>
         <v>950256603.21205628</v>
       </c>
-      <c r="C175" s="7">
+      <c r="C175" s="6">
         <f t="shared" si="18"/>
         <v>470699309.18473428</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" s="7">
+    <row r="176" spans="1:4">
+      <c r="A176" s="6">
         <f t="shared" si="17"/>
         <v>961779169.24417686</v>
       </c>
-      <c r="C176" s="7">
+      <c r="C176" s="6">
         <f t="shared" si="18"/>
         <v>472699309.18473428</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A177" s="7">
+    <row r="177" spans="1:6">
+      <c r="A177" s="6">
         <f t="shared" si="17"/>
         <v>973416960.93661869</v>
       </c>
-      <c r="C177" s="7">
+      <c r="C177" s="6">
         <f t="shared" si="18"/>
         <v>474699309.18473428</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="7">
+    <row r="178" spans="1:6">
+      <c r="A178" s="6">
         <f t="shared" si="17"/>
         <v>985171130.54598486</v>
       </c>
-      <c r="C178" s="7">
+      <c r="C178" s="6">
         <f t="shared" si="18"/>
         <v>476699309.18473428</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A179" s="7">
+    <row r="179" spans="1:6">
+      <c r="A179" s="6">
         <f t="shared" si="17"/>
         <v>997042841.85144472</v>
       </c>
-      <c r="C179" s="7">
+      <c r="C179" s="6">
         <f t="shared" si="18"/>
         <v>478699309.18473428</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="7">
+    <row r="180" spans="1:6">
+      <c r="A180" s="6">
         <f t="shared" si="17"/>
         <v>1009033270.2699592</v>
       </c>
-      <c r="B180" s="7">
+      <c r="B180" s="6">
         <v>15</v>
       </c>
-      <c r="C180" s="7">
+      <c r="C180" s="6">
         <f>(C179+F$2)*D180</f>
         <v>499927281.55212367</v>
       </c>
-      <c r="D180" s="3">
+      <c r="D180" s="2">
         <v>1.04</v>
       </c>
-      <c r="F180" s="7" t="s">
-        <v>31</v>
+      <c r="F180" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GitHub / RobomationLAB / BeagleAPI_KR 내용 기입 완료, 대항목별 설명 필요, SideBar 미완
</commit_message>
<xml_diff>
--- a/PIO_check/PIO_SCRATCH.xlsx
+++ b/PIO_check/PIO_SCRATCH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imseongsu/robomation/personal_tjdtn/PIO_check/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robomation_TUF15\personal_tjdtn\PIO_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB78A4E2-F349-1F44-B22A-2FDFCE63CC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01319424-2586-4646-80F5-7056791F62EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1940" windowWidth="23240" windowHeight="12820" xr2:uid="{385024C5-CB96-4C20-A0A9-1BB6D9BF6AC5}"/>
+    <workbookView xWindow="3840" yWindow="1965" windowWidth="23235" windowHeight="12825" xr2:uid="{385024C5-CB96-4C20-A0A9-1BB6D9BF6AC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>CMA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,10 +142,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>월 2%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>목표</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -159,10 +155,6 @@
   </si>
   <si>
     <t>금리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>15년차에 두배차이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -189,6 +181,10 @@
     <t>GOOGL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>월 5%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -198,7 +194,7 @@
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,35 +377,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1471,6 +1439,341 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ko-KR" altLang="en-US"/>
+              <a:t>차이 배율</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ko-KR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet2!$F$13,Sheet2!$F$24,Sheet2!$F$36,Sheet2!$F$48,Sheet2!$F$60,Sheet2!$F$72,Sheet2!$F$84,Sheet2!$F$96,Sheet2!$F$108,Sheet2!$F$120,Sheet2!$F$132,Sheet2!$F$144,Sheet2!$F$156,Sheet2!$F$168,Sheet2!$F$180)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00_ </c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.3756104921952319</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8400561271542561</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5986699809885443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7590646106110057</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5576584916267864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3771111364146407</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.840642082653607</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.968286484559417</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.436828454443035</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50.013424342429545</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80.280762961111151</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>129.85249689352446</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>211.41461639459661</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>346.1605554655942</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>569.58174496765093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BE5-48E2-B6CD-0E18D7AFD74A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1404630367"/>
+        <c:axId val="1404630847"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1404630367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404630847"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1404630847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404630367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1631,6 +1934,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -3675,6 +4018,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3856,6 +4702,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7207435-544A-80F8-72D3-1C9439CAD6DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4227,33 +5114,33 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1">
-        <v>1336.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+        <v>1341.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -4300,26 +5187,26 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C4">
-        <v>15.38</v>
+        <v>760.76</v>
       </c>
       <c r="D4">
-        <v>15.38</v>
+        <v>760.76</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="6">
         <f>C4*D1</f>
-        <v>20549.218000000001</v>
+        <v>1020863.844</v>
       </c>
       <c r="L4" s="6">
         <f>D4*D1</f>
-        <v>20549.218000000001</v>
+        <v>1020863.844</v>
       </c>
       <c r="Q4" t="s">
         <v>5</v>
@@ -4331,7 +5218,7 @@
         <v>1.0123</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -4363,15 +5250,15 @@
       </c>
       <c r="L5" s="6">
         <f>D5*D1</f>
-        <v>236489.69999999998</v>
+        <v>237516.30000000002</v>
       </c>
       <c r="M5" s="6">
         <f>L5-K5</f>
-        <v>-824.30000000001746</v>
+        <v>202.30000000001746</v>
       </c>
       <c r="N5" s="7">
         <f>(L5/K5-1)</f>
-        <v>-3.4734571074610532E-3</v>
+        <v>8.5245708217818184E-4</v>
       </c>
       <c r="Q5" t="s">
         <v>1</v>
@@ -4383,7 +5270,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -4415,15 +5302,15 @@
       </c>
       <c r="L6" s="6">
         <f>D6*D1</f>
-        <v>571302.99899999995</v>
+        <v>573783.02099999995</v>
       </c>
       <c r="M6" s="6">
         <f>L6-K6</f>
-        <v>30129.998999999953</v>
+        <v>32610.02099999995</v>
       </c>
       <c r="N6" s="7">
         <f>(L6/K6-1)</f>
-        <v>5.5675355200647481E-2</v>
+        <v>6.0258033937391486E-2</v>
       </c>
       <c r="Q6" t="s">
         <v>23</v>
@@ -4435,7 +5322,7 @@
         <v>-1.09E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -4467,127 +5354,184 @@
       </c>
       <c r="L7" s="6">
         <f>D7*D1</f>
-        <v>1262080.06</v>
+        <v>1267558.7400000002</v>
       </c>
       <c r="M7" s="6">
         <f>L7-K7</f>
-        <v>349632.06000000006</v>
+        <v>355110.74000000022</v>
       </c>
       <c r="N7" s="7">
         <f>(L7/K7-1)</f>
-        <v>0.38318025794346644</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+        <v>0.38918463298730477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2">
         <f>SUM(C4:C7)</f>
-        <v>1281.9099999999999</v>
+        <v>2027.29</v>
       </c>
       <c r="D8" s="2">
         <f>SUM(D4:D7)</f>
-        <v>1564.5700000000002</v>
+        <v>2309.9499999999998</v>
       </c>
       <c r="E8" s="2">
         <f>D8-C8</f>
-        <v>282.66000000000031</v>
+        <v>282.65999999999985</v>
       </c>
       <c r="F8" s="7">
         <f>(D8/C8-1)</f>
-        <v>0.22049909900071007</v>
+        <v>0.13942751160416123</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="6">
         <f>SUM(K4:K7)</f>
-        <v>1711484.2179999999</v>
+        <v>2711798.844</v>
       </c>
       <c r="L8" s="6">
         <f>SUM(L4:L7)</f>
-        <v>2090421.977</v>
+        <v>3099721.9050000003</v>
       </c>
       <c r="M8" s="6">
         <f>L8-K8</f>
-        <v>378937.75900000008</v>
+        <v>387923.06100000022</v>
       </c>
       <c r="N8" s="7">
         <f>(L8/K8-1)</f>
-        <v>0.22140885379756403</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
+        <v>0.14305008716199619</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L12" t="s">
         <v>24</v>
       </c>
       <c r="M12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="K14" s="6"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K14" s="6">
+        <v>2000000</v>
+      </c>
       <c r="L14" s="13">
         <v>2061812</v>
       </c>
       <c r="M14" s="14">
         <v>45375</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="6">
         <v>2088860</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="O14">
+        <f>N14/K14</f>
+        <v>1.04443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K15" s="6">
+        <f>K14+1000000</f>
+        <v>3000000</v>
+      </c>
       <c r="L15" s="13">
-        <f>(L14+1000000)*1.02</f>
-        <v>3123048.24</v>
+        <f>(L14+1000000)*1.05</f>
+        <v>3214902.6</v>
       </c>
       <c r="M15" s="14">
         <v>45406</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="N15" s="13">
+        <f>(N14+1000000)*1.05</f>
+        <v>3243303</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15:O18" si="0">N15/K15</f>
+        <v>1.0811010000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K16" s="6">
+        <f t="shared" ref="K16:K18" si="1">K15+1000000</f>
+        <v>4000000</v>
+      </c>
       <c r="L16" s="13">
-        <f t="shared" ref="L16:L18" si="0">(L15+1000000)*1.02</f>
-        <v>4205509.2048000004</v>
+        <f t="shared" ref="L16:L18" si="2">(L15+1000000)*1.05</f>
+        <v>4425647.7299999995</v>
       </c>
       <c r="M16" s="14">
         <v>45436</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="N16" s="13">
+        <f t="shared" ref="N16:N18" si="3">(N15+1000000)*1.05</f>
+        <v>4455468.1500000004</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>1.1138670375000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K17" s="6">
+        <f t="shared" si="1"/>
+        <v>5000000</v>
+      </c>
       <c r="L17" s="13">
-        <f t="shared" si="0"/>
-        <v>5309619.3888960006</v>
+        <f t="shared" si="2"/>
+        <v>5696930.1164999995</v>
       </c>
       <c r="M17" s="14">
         <v>45467</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="N17" s="13">
+        <f t="shared" si="3"/>
+        <v>5728241.557500001</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>1.1456483115000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K18" s="6">
+        <f t="shared" si="1"/>
+        <v>6000000</v>
+      </c>
       <c r="L18" s="13">
-        <f t="shared" si="0"/>
-        <v>6435811.7766739205</v>
+        <f t="shared" si="2"/>
+        <v>7031776.6223249994</v>
       </c>
       <c r="M18" s="14">
         <v>45497</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="N18" s="13">
+        <f t="shared" si="3"/>
+        <v>7064653.6353750015</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>1.1774422725625002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="P19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G20" s="6">
         <v>600000</v>
       </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
       <c r="J20" t="s">
         <v>19</v>
       </c>
@@ -4597,7 +5541,7 @@
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="19" t="s">
         <v>18</v>
@@ -4618,16 +5562,16 @@
         <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K21" s="16">
         <v>600000</v>
       </c>
       <c r="P21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>45372</v>
       </c>
@@ -4650,29 +5594,32 @@
       <c r="G22" s="6">
         <v>304595</v>
       </c>
+      <c r="H22" s="6">
+        <v>1333</v>
+      </c>
       <c r="J22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K22" s="16">
         <v>23190</v>
       </c>
       <c r="P22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q22">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>45376</v>
       </c>
       <c r="B23" s="6">
-        <f t="shared" ref="B23" si="1">SUM(C23:G23)</f>
+        <f t="shared" ref="B23" si="4">SUM(C23:G23)</f>
         <v>4319086</v>
       </c>
       <c r="C23" s="6">
-        <v>2093224</v>
+        <v>3093224</v>
       </c>
       <c r="D23" s="6">
         <v>214865</v>
@@ -4684,17 +5631,21 @@
         <v>30207</v>
       </c>
       <c r="G23" s="6">
-        <v>1879795</v>
+        <v>879795</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1342</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K23" s="16">
         <f>K20-K21-K22</f>
         <v>1020710</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -4702,6 +5653,10 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
+      <c r="M24">
+        <f>D4+M23</f>
+        <v>760.76</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4722,6 +5677,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B22:B23" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4730,22 +5688,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1629F0B6-94E5-4505-A80D-FDBB4E358C97}">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F177" sqref="F177"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="6" customWidth="1"/>
     <col min="2" max="2" width="9" style="6"/>
-    <col min="3" max="3" width="13.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="6" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="6" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6">
         <f>F2</f>
         <v>2000000</v>
@@ -4756,20 +5715,20 @@
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <f>(A1+F2)*G2</f>
-        <v>4040000</v>
+        <v>4200000</v>
       </c>
       <c r="C2" s="6">
         <f>C1+F$2</f>
@@ -4782,1887 +5741,1960 @@
         <v>2000000</v>
       </c>
       <c r="G2" s="2">
-        <v>1.01</v>
+        <v>1.05</v>
       </c>
       <c r="H2" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>1.0349999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>(A2+F$2)*G$2</f>
-        <v>6100400</v>
+        <v>6510000</v>
       </c>
       <c r="C3" s="6">
         <f>C2+F$2</f>
         <v>6000000</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f>(A3+F$2)*G$2</f>
-        <v>8181404</v>
+        <v>8935500</v>
       </c>
       <c r="C4" s="6">
         <f t="shared" ref="C4:C12" si="0">C3+F$2</f>
         <v>8000000</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <f t="shared" ref="A5:A68" si="1">(A4+F$2)*G$2</f>
-        <v>10283218.040000001</v>
+        <v>11482275</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <f t="shared" si="1"/>
-        <v>12406050.220400002</v>
+        <v>14156388.75</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>12000000</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <f t="shared" si="1"/>
-        <v>14550110.722604003</v>
+        <v>16964208.1875</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>14000000</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <f t="shared" si="1"/>
-        <v>16715611.829830043</v>
+        <v>19912418.596875001</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>16000000</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <f t="shared" si="1"/>
-        <v>18902767.948128343</v>
+        <v>23008039.526718751</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>18000000</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <f t="shared" si="1"/>
-        <v>21111795.627609625</v>
+        <v>26258441.50305469</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>20000000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <f t="shared" si="1"/>
-        <v>23342913.583885722</v>
+        <v>29671363.578207426</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>22000000</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <f t="shared" si="1"/>
-        <v>25596342.719724581</v>
+        <v>33254931.757117797</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
         <v>24000000</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="1"/>
-        <v>27872306.146921828</v>
+        <v>37017678.344973683</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
       </c>
       <c r="C13" s="6">
         <f>(C12+F$2)*D13</f>
-        <v>27040000</v>
+        <v>26909999.999999996</v>
       </c>
       <c r="D13" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <f>A13/C13</f>
+        <v>1.3756104921952319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="1"/>
-        <v>30171029.208391048</v>
+        <v>40968562.262222372</v>
       </c>
       <c r="C14" s="6">
         <f>C13+F$2</f>
-        <v>29040000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>28909999.999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="1"/>
-        <v>32492739.50047496</v>
+        <v>45116990.375333495</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" ref="C15:C23" si="2">C14+F$2</f>
-        <v>31040000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>30909999.999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="1"/>
-        <v>34837666.895479709</v>
+        <v>49472839.894100174</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="2"/>
-        <v>33040000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>32909999.999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="1"/>
-        <v>37206043.564434506</v>
+        <v>54046481.888805188</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="2"/>
-        <v>35040000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>34910000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="1"/>
-        <v>39598104.000078849</v>
+        <v>58848805.983245447</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="2"/>
-        <v>37040000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>36910000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="1"/>
-        <v>42014085.040079638</v>
+        <v>63891246.282407723</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="2"/>
-        <v>39040000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>38910000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
-        <v>44454225.890480436</v>
+        <v>69185808.596528113</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="2"/>
-        <v>41040000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>40910000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <f t="shared" si="1"/>
-        <v>46918768.149385244</v>
+        <v>74745099.026354522</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="2"/>
-        <v>43040000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>42910000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <f t="shared" si="1"/>
-        <v>49407955.8308791</v>
+        <v>80582353.977672249</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="2"/>
-        <v>45040000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>44910000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <f t="shared" si="1"/>
-        <v>51922035.389187895</v>
+        <v>86711471.676555872</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="2"/>
-        <v>47040000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>46910000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <f t="shared" si="1"/>
-        <v>54461255.743079774</v>
+        <v>93147045.260383666</v>
       </c>
       <c r="B24" s="6">
         <v>2</v>
       </c>
       <c r="C24" s="6">
         <f>(C23+F$2)*D24</f>
-        <v>51001600</v>
+        <v>50621849.999999993</v>
       </c>
       <c r="D24" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F24" s="2">
+        <f>A24/C24</f>
+        <v>1.8400561271542561</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <f t="shared" si="1"/>
-        <v>57025868.30051057</v>
+        <v>99904397.523402855</v>
       </c>
       <c r="C25" s="6">
         <f>C24+F$2</f>
-        <v>53001600</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>52621849.999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <f t="shared" si="1"/>
-        <v>59616126.98351568</v>
+        <v>106999617.399573</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" ref="C26:C35" si="3">C25+F$2</f>
-        <v>55001600</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>54621849.999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <f t="shared" si="1"/>
-        <v>62232288.253350839</v>
+        <v>114449598.26955165</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="3"/>
-        <v>57001600</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>56621849.999999993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <f t="shared" si="1"/>
-        <v>64874611.135884345</v>
+        <v>122272078.18302923</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="3"/>
-        <v>59001600</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>58621849.999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <f t="shared" si="1"/>
-        <v>67543357.247243196</v>
+        <v>130485682.0921807</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="3"/>
-        <v>61001600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>60621849.999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <f t="shared" si="1"/>
-        <v>70238790.819715634</v>
+        <v>139109966.19678974</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" si="3"/>
-        <v>63001600</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>62621849.999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <f t="shared" si="1"/>
-        <v>72961178.727912784</v>
+        <v>148165464.50662923</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" si="3"/>
-        <v>65001600</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>64621849.999999993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <f t="shared" si="1"/>
-        <v>75710790.515191913</v>
+        <v>157673737.73196068</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" si="3"/>
-        <v>67001600</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>66621849.999999993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <f t="shared" si="1"/>
-        <v>78487898.420343831</v>
+        <v>167657424.61855873</v>
       </c>
       <c r="C33" s="6">
         <f t="shared" si="3"/>
-        <v>69001600</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>68621850</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <f t="shared" si="1"/>
-        <v>81292777.404547274</v>
+        <v>178140295.84948668</v>
       </c>
       <c r="C34" s="6">
         <f t="shared" si="3"/>
-        <v>71001600</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>70621850</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <f t="shared" si="1"/>
-        <v>84125705.178592741</v>
+        <v>189147310.64196101</v>
       </c>
       <c r="C35" s="6">
         <f t="shared" si="3"/>
-        <v>73001600</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>72621850</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <f t="shared" si="1"/>
-        <v>86986962.230378672</v>
+        <v>200704676.17405906</v>
       </c>
       <c r="B36" s="6">
         <v>3</v>
       </c>
       <c r="C36" s="6">
         <f>(C35+F$2)*D36</f>
-        <v>78001664</v>
+        <v>77233614.75</v>
       </c>
       <c r="D36" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F36" s="2">
+        <f>A36/C36</f>
+        <v>2.5986699809885443</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <f t="shared" si="1"/>
-        <v>89876831.852682456</v>
+        <v>212839909.98276204</v>
       </c>
       <c r="C37" s="6">
         <f>C36+F$2</f>
-        <v>80001664</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>79233614.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <f t="shared" si="1"/>
-        <v>92795600.171209276</v>
+        <v>225581905.48190016</v>
       </c>
       <c r="C38" s="6">
         <f t="shared" ref="C38:C47" si="4">C37+F$2</f>
-        <v>82001664</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>81233614.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <f t="shared" si="1"/>
-        <v>95743556.172921374</v>
+        <v>238961000.75599518</v>
       </c>
       <c r="C39" s="6">
         <f t="shared" si="4"/>
-        <v>84001664</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>83233614.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <f t="shared" si="1"/>
-        <v>98720991.734650582</v>
+        <v>253009050.79379496</v>
       </c>
       <c r="C40" s="6">
         <f t="shared" si="4"/>
-        <v>86001664</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>85233614.75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <f t="shared" si="1"/>
-        <v>101728201.65199709</v>
+        <v>267759503.33348471</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" si="4"/>
-        <v>88001664</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>87233614.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <f t="shared" si="1"/>
-        <v>104765483.66851707</v>
+        <v>283247478.50015897</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="4"/>
-        <v>90001664</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>89233614.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <f t="shared" si="1"/>
-        <v>107833138.50520223</v>
+        <v>299509852.4251669</v>
       </c>
       <c r="C43" s="6">
         <f t="shared" si="4"/>
-        <v>92001664</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>91233614.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <f t="shared" si="1"/>
-        <v>110931469.89025426</v>
+        <v>316585345.04642528</v>
       </c>
       <c r="C44" s="6">
         <f t="shared" si="4"/>
-        <v>94001664</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>93233614.75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <f t="shared" si="1"/>
-        <v>114060784.58915681</v>
+        <v>334514612.29874659</v>
       </c>
       <c r="C45" s="6">
         <f t="shared" si="4"/>
-        <v>96001664</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>95233614.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <f t="shared" si="1"/>
-        <v>117221392.43504837</v>
+        <v>353340342.91368395</v>
       </c>
       <c r="C46" s="6">
         <f t="shared" si="4"/>
-        <v>98001664</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>97233614.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <f t="shared" si="1"/>
-        <v>120413606.35939886</v>
+        <v>373107360.05936819</v>
       </c>
       <c r="C47" s="6">
         <f t="shared" si="4"/>
-        <v>100001664</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>99233614.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <f t="shared" si="1"/>
-        <v>123637742.42299284</v>
+        <v>393862728.06233662</v>
       </c>
       <c r="B48" s="6">
         <v>4</v>
       </c>
       <c r="C48" s="6">
         <f>(C47+F$2)*D48</f>
-        <v>106081730.56</v>
+        <v>104776791.26624998</v>
       </c>
       <c r="D48" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F48" s="2">
+        <f>A48/C48</f>
+        <v>3.7590646106110057</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <f t="shared" si="1"/>
-        <v>126894119.84722278</v>
+        <v>415655864.46545345</v>
       </c>
       <c r="C49" s="6">
         <f>C48+F$2</f>
-        <v>108081730.56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>106776791.26624998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <f t="shared" si="1"/>
-        <v>130183061.04569501</v>
+        <v>438538657.68872613</v>
       </c>
       <c r="C50" s="6">
         <f t="shared" ref="C50:C59" si="5">C49+F$2</f>
-        <v>110081730.56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>108776791.26624998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <f t="shared" si="1"/>
-        <v>133504891.65615197</v>
+        <v>462565590.57316244</v>
       </c>
       <c r="C51" s="6">
         <f t="shared" si="5"/>
-        <v>112081730.56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>110776791.26624998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <f t="shared" si="1"/>
-        <v>136859940.57271346</v>
+        <v>487793870.10182059</v>
       </c>
       <c r="C52" s="6">
         <f t="shared" si="5"/>
-        <v>114081730.56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>112776791.26624998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <f t="shared" si="1"/>
-        <v>140248539.97844061</v>
+        <v>514283563.60691166</v>
       </c>
       <c r="C53" s="6">
         <f t="shared" si="5"/>
-        <v>116081730.56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>114776791.26624998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <f t="shared" si="1"/>
-        <v>143671025.37822503</v>
+        <v>542097741.78725731</v>
       </c>
       <c r="C54" s="6">
         <f t="shared" si="5"/>
-        <v>118081730.56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>116776791.26624998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <f t="shared" si="1"/>
-        <v>147127735.63200727</v>
+        <v>571302628.87662017</v>
       </c>
       <c r="C55" s="6">
         <f t="shared" si="5"/>
-        <v>120081730.56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>118776791.26624998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <f t="shared" si="1"/>
-        <v>150619012.98832735</v>
+        <v>601967760.32045126</v>
       </c>
       <c r="C56" s="6">
         <f t="shared" si="5"/>
-        <v>122081730.56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>120776791.26624998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <f t="shared" si="1"/>
-        <v>154145203.11821064</v>
+        <v>634166148.33647382</v>
       </c>
       <c r="C57" s="6">
         <f t="shared" si="5"/>
-        <v>124081730.56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>122776791.26624998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <f t="shared" si="1"/>
-        <v>157706655.14939275</v>
+        <v>667974455.75329757</v>
       </c>
       <c r="C58" s="6">
         <f t="shared" si="5"/>
-        <v>126081730.56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>124776791.26624998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <f t="shared" si="1"/>
-        <v>161303721.7008867</v>
+        <v>703473178.54096246</v>
       </c>
       <c r="C59" s="6">
         <f t="shared" si="5"/>
-        <v>128081730.56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>126776791.26624998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <f t="shared" si="1"/>
-        <v>164936758.91789556</v>
+        <v>740746837.46801066</v>
       </c>
       <c r="B60" s="6">
         <v>5</v>
       </c>
       <c r="C60" s="6">
         <f>(C59+F$2)*D60</f>
-        <v>135284999.78240001</v>
+        <v>133283978.96056873</v>
       </c>
       <c r="D60" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F60" s="2">
+        <f>A60/C60</f>
+        <v>5.5576584916267864</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <f t="shared" si="1"/>
-        <v>168606126.50707451</v>
+        <v>779884179.34141123</v>
       </c>
       <c r="C61" s="6">
         <f>C60+F$2</f>
-        <v>137284999.78240001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>135283978.96056873</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <f t="shared" si="1"/>
-        <v>172312187.77214524</v>
+        <v>820978388.30848181</v>
       </c>
       <c r="C62" s="6">
         <f t="shared" ref="C62:C71" si="6">C61+F$2</f>
-        <v>139284999.78240001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>137283978.96056873</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <f t="shared" si="1"/>
-        <v>176055309.6498667</v>
+        <v>864127307.72390592</v>
       </c>
       <c r="C63" s="6">
         <f t="shared" si="6"/>
-        <v>141284999.78240001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>139283978.96056873</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <f t="shared" si="1"/>
-        <v>179835862.74636537</v>
+        <v>909433673.11010122</v>
       </c>
       <c r="C64" s="6">
         <f t="shared" si="6"/>
-        <v>143284999.78240001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>141283978.96056873</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <f t="shared" si="1"/>
-        <v>183654221.37382904</v>
+        <v>957005356.76560628</v>
       </c>
       <c r="C65" s="6">
         <f t="shared" si="6"/>
-        <v>145284999.78240001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>143283978.96056873</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <f t="shared" si="1"/>
-        <v>187510763.58756733</v>
+        <v>1006955624.6038866</v>
       </c>
       <c r="C66" s="6">
         <f t="shared" si="6"/>
-        <v>147284999.78240001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>145283978.96056873</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <f t="shared" si="1"/>
-        <v>191405871.223443</v>
+        <v>1059403405.8340809</v>
       </c>
       <c r="C67" s="6">
         <f t="shared" si="6"/>
-        <v>149284999.78240001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>147283978.96056873</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <f t="shared" si="1"/>
-        <v>195339929.93567744</v>
+        <v>1114473576.1257851</v>
       </c>
       <c r="C68" s="6">
         <f t="shared" si="6"/>
-        <v>151284999.78240001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>149283978.96056873</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <f t="shared" ref="A69:A132" si="7">(A68+F$2)*G$2</f>
-        <v>199313329.23503423</v>
+        <v>1172297254.9320743</v>
       </c>
       <c r="C69" s="6">
         <f t="shared" si="6"/>
-        <v>153284999.78240001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>151283978.96056873</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <f t="shared" si="7"/>
-        <v>203326462.52738458</v>
+        <v>1233012117.678678</v>
       </c>
       <c r="C70" s="6">
         <f t="shared" si="6"/>
-        <v>155284999.78240001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>153283978.96056873</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <f t="shared" si="7"/>
-        <v>207379727.15265843</v>
+        <v>1296762723.5626121</v>
       </c>
       <c r="C71" s="6">
         <f t="shared" si="6"/>
-        <v>157284999.78240001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>155283978.96056873</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <f t="shared" si="7"/>
-        <v>211473524.42418501</v>
+        <v>1363700859.7407427</v>
       </c>
       <c r="B72" s="6">
         <v>6</v>
       </c>
       <c r="C72" s="6">
         <f>(C71+F$2)*D72</f>
-        <v>165656399.77369601</v>
+        <v>162788918.22418863</v>
       </c>
       <c r="D72" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F72" s="2">
+        <f>A72/C72</f>
+        <v>8.3771111364146407</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <f t="shared" si="7"/>
-        <v>215608259.66842687</v>
+        <v>1433985902.7277799</v>
       </c>
       <c r="C73" s="6">
         <f>C72+F$2</f>
-        <v>167656399.77369601</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>164788918.22418863</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <f t="shared" si="7"/>
-        <v>219784342.26511115</v>
+        <v>1507785197.8641689</v>
       </c>
       <c r="C74" s="6">
         <f t="shared" ref="C74:C83" si="8">C73+F$2</f>
-        <v>169656399.77369601</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>166788918.22418863</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <f t="shared" si="7"/>
-        <v>224002185.68776226</v>
+        <v>1585274457.7573774</v>
       </c>
       <c r="C75" s="6">
         <f t="shared" si="8"/>
-        <v>171656399.77369601</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>168788918.22418863</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <f t="shared" si="7"/>
-        <v>228262207.54463989</v>
+        <v>1666638180.6452463</v>
       </c>
       <c r="C76" s="6">
         <f t="shared" si="8"/>
-        <v>173656399.77369601</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>170788918.22418863</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <f t="shared" si="7"/>
-        <v>232564829.62008628</v>
+        <v>1752070089.6775086</v>
       </c>
       <c r="C77" s="6">
         <f t="shared" si="8"/>
-        <v>175656399.77369601</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>172788918.22418863</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <f t="shared" si="7"/>
-        <v>236910477.91628715</v>
+        <v>1841773594.1613841</v>
       </c>
       <c r="C78" s="6">
         <f t="shared" si="8"/>
-        <v>177656399.77369601</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>174788918.22418863</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <f t="shared" si="7"/>
-        <v>241299582.69545004</v>
+        <v>1935962273.8694534</v>
       </c>
       <c r="C79" s="6">
         <f t="shared" si="8"/>
-        <v>179656399.77369601</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>176788918.22418863</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <f t="shared" si="7"/>
-        <v>245732578.52240455</v>
+        <v>2034860387.5629263</v>
       </c>
       <c r="C80" s="6">
         <f t="shared" si="8"/>
-        <v>181656399.77369601</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>178788918.22418863</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <f t="shared" si="7"/>
-        <v>250209904.3076286</v>
+        <v>2138703406.9410727</v>
       </c>
       <c r="C81" s="6">
         <f t="shared" si="8"/>
-        <v>183656399.77369601</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>180788918.22418863</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <f t="shared" si="7"/>
-        <v>254732003.35070488</v>
+        <v>2247738577.2881265</v>
       </c>
       <c r="C82" s="6">
         <f t="shared" si="8"/>
-        <v>185656399.77369601</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>182788918.22418863</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <f t="shared" si="7"/>
-        <v>259299323.38421193</v>
+        <v>2362225506.1525331</v>
       </c>
       <c r="C83" s="6">
         <f t="shared" si="8"/>
-        <v>187656399.77369601</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>184788918.22418863</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <f t="shared" si="7"/>
-        <v>263912316.61805406</v>
+        <v>2482436781.4601598</v>
       </c>
       <c r="B84" s="6">
         <v>7</v>
       </c>
       <c r="C84" s="6">
         <f>(C83+F$2)*D84</f>
-        <v>197242655.76464385</v>
+        <v>193326530.36203521</v>
       </c>
       <c r="D84" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F84" s="2">
+        <f>A84/C84</f>
+        <v>12.840642082653607</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <f t="shared" si="7"/>
-        <v>268571439.78423458</v>
+        <v>2608658620.5331678</v>
       </c>
       <c r="C85" s="6">
         <f>C84+F$2</f>
-        <v>199242655.76464385</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>195326530.36203521</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <f t="shared" si="7"/>
-        <v>273277154.18207693</v>
+        <v>2741191551.5598264</v>
       </c>
       <c r="C86" s="6">
         <f t="shared" ref="C86:C95" si="9">C85+F$2</f>
-        <v>201242655.76464385</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>197326530.36203521</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <f t="shared" si="7"/>
-        <v>278029925.7238977</v>
+        <v>2880351129.1378179</v>
       </c>
       <c r="C87" s="6">
         <f t="shared" si="9"/>
-        <v>203242655.76464385</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>199326530.36203521</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <f t="shared" si="7"/>
-        <v>282830224.98113668</v>
+        <v>3026468685.5947089</v>
       </c>
       <c r="C88" s="6">
         <f t="shared" si="9"/>
-        <v>205242655.76464385</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>201326530.36203521</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <f t="shared" si="7"/>
-        <v>287678527.23094803</v>
+        <v>3179892119.8744445</v>
       </c>
       <c r="C89" s="6">
         <f t="shared" si="9"/>
-        <v>207242655.76464385</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>203326530.36203521</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <f t="shared" si="7"/>
-        <v>292575312.50325751</v>
+        <v>3340986725.8681669</v>
       </c>
       <c r="C90" s="6">
         <f t="shared" si="9"/>
-        <v>209242655.76464385</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>205326530.36203521</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <f t="shared" si="7"/>
-        <v>297521065.62829012</v>
+        <v>3510136062.1615753</v>
       </c>
       <c r="C91" s="6">
         <f t="shared" si="9"/>
-        <v>211242655.76464385</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>207326530.36203521</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <f t="shared" si="7"/>
-        <v>302516276.28457302</v>
+        <v>3687742865.2696543</v>
       </c>
       <c r="C92" s="6">
         <f t="shared" si="9"/>
-        <v>213242655.76464385</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>209326530.36203521</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <f t="shared" si="7"/>
-        <v>307561439.04741877</v>
+        <v>3874230008.5331373</v>
       </c>
       <c r="C93" s="6">
         <f t="shared" si="9"/>
-        <v>215242655.76464385</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>211326530.36203521</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <f t="shared" si="7"/>
-        <v>312657053.43789297</v>
+        <v>4070041508.9597945</v>
       </c>
       <c r="C94" s="6">
         <f t="shared" si="9"/>
-        <v>217242655.76464385</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>213326530.36203521</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <f t="shared" si="7"/>
-        <v>317803623.97227192</v>
+        <v>4275643584.4077845</v>
       </c>
       <c r="C95" s="6">
         <f t="shared" si="9"/>
-        <v>219242655.76464385</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
+        <v>215326530.36203521</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <f t="shared" si="7"/>
-        <v>323001660.21199465</v>
+        <v>4491525763.6281738</v>
       </c>
       <c r="B96" s="6">
         <v>8</v>
       </c>
       <c r="C96" s="6">
         <f>(C95+F$2)*D96</f>
-        <v>230092361.9952296</v>
+        <v>224932958.92470643</v>
       </c>
       <c r="D96" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F96" s="2">
+        <f>A96/C96</f>
+        <v>19.968286484559417</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <f t="shared" si="7"/>
-        <v>328251676.81411457</v>
+        <v>4718202051.8095827</v>
       </c>
       <c r="C97" s="6">
         <f>C96+F$2</f>
-        <v>232092361.9952296</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>226932958.92470643</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <f t="shared" si="7"/>
-        <v>333554193.58225572</v>
+        <v>4956212154.4000616</v>
       </c>
       <c r="C98" s="6">
         <f t="shared" ref="C98:C107" si="10">C97+F$2</f>
-        <v>234092361.9952296</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>228932958.92470643</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <f t="shared" si="7"/>
-        <v>338909735.51807827</v>
+        <v>5206122762.1200647</v>
       </c>
       <c r="C99" s="6">
         <f t="shared" si="10"/>
-        <v>236092361.9952296</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>230932958.92470643</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <f t="shared" si="7"/>
-        <v>344318832.87325907</v>
+        <v>5468528900.2260685</v>
       </c>
       <c r="C100" s="6">
         <f t="shared" si="10"/>
-        <v>238092361.9952296</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>232932958.92470643</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <f t="shared" si="7"/>
-        <v>349782021.20199168</v>
+        <v>5744055345.2373724</v>
       </c>
       <c r="C101" s="6">
         <f t="shared" si="10"/>
-        <v>240092361.9952296</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>234932958.92470643</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <f t="shared" si="7"/>
-        <v>355299841.4140116</v>
+        <v>6033358112.4992409</v>
       </c>
       <c r="C102" s="6">
         <f t="shared" si="10"/>
-        <v>242092361.9952296</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>236932958.92470643</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <f t="shared" si="7"/>
-        <v>360872839.8281517</v>
+        <v>6337126018.1242027</v>
       </c>
       <c r="C103" s="6">
         <f t="shared" si="10"/>
-        <v>244092361.9952296</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+        <v>238932958.92470643</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <f t="shared" si="7"/>
-        <v>366501568.22643322</v>
+        <v>6656082319.0304127</v>
       </c>
       <c r="C104" s="6">
         <f t="shared" si="10"/>
-        <v>246092361.9952296</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>240932958.92470643</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <f t="shared" si="7"/>
-        <v>372186583.90869755</v>
+        <v>6990986434.9819336</v>
       </c>
       <c r="C105" s="6">
         <f t="shared" si="10"/>
-        <v>248092361.9952296</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>242932958.92470643</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <f t="shared" si="7"/>
-        <v>377928449.7477845</v>
+        <v>7342635756.7310305</v>
       </c>
       <c r="C106" s="6">
         <f t="shared" si="10"/>
-        <v>250092361.9952296</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
+        <v>244932958.92470643</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <f t="shared" si="7"/>
-        <v>383727734.24526232</v>
+        <v>7711867544.5675821</v>
       </c>
       <c r="C107" s="6">
         <f t="shared" si="10"/>
-        <v>252092361.9952296</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
+        <v>246932958.92470643</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <f t="shared" si="7"/>
-        <v>389585011.58771497</v>
+        <v>8099560921.7959614</v>
       </c>
       <c r="B108" s="6">
         <v>9</v>
       </c>
       <c r="C108" s="6">
         <f>(C107+F$2)*D108</f>
-        <v>264256056.4750388</v>
+        <v>257645612.48707113</v>
       </c>
       <c r="D108" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F108" s="2">
+        <f>A108/C108</f>
+        <v>31.436828454443035</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
         <f t="shared" si="7"/>
-        <v>395500861.70359212</v>
+        <v>8506638967.8857594</v>
       </c>
       <c r="C109" s="6">
         <f>C108+F$2</f>
-        <v>266256056.4750388</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>259645612.48707113</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
         <f t="shared" si="7"/>
-        <v>401475870.32062805</v>
+        <v>8934070916.2800484</v>
       </c>
       <c r="C110" s="6">
         <f t="shared" ref="C110:C119" si="11">C109+F$2</f>
-        <v>268256056.4750388</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
+        <v>261645612.48707113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
         <f t="shared" si="7"/>
-        <v>407510629.02383435</v>
+        <v>9382874462.0940514</v>
       </c>
       <c r="C111" s="6">
         <f t="shared" si="11"/>
-        <v>270256056.47503877</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
+        <v>263645612.48707113</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
         <f t="shared" si="7"/>
-        <v>413605735.31407267</v>
+        <v>9854118185.1987553</v>
       </c>
       <c r="C112" s="6">
         <f t="shared" si="11"/>
-        <v>272256056.47503877</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
+        <v>265645612.48707113</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
         <f t="shared" si="7"/>
-        <v>419761792.66721338</v>
+        <v>10348924094.458693</v>
       </c>
       <c r="C113" s="6">
         <f t="shared" si="11"/>
-        <v>274256056.47503877</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
+        <v>267645612.48707113</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
         <f t="shared" si="7"/>
-        <v>425979410.59388554</v>
+        <v>10868470299.181627</v>
       </c>
       <c r="C114" s="6">
         <f t="shared" si="11"/>
-        <v>276256056.47503877</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
+        <v>269645612.48707116</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
         <f t="shared" si="7"/>
-        <v>432259204.69982439</v>
+        <v>11413993814.140709</v>
       </c>
       <c r="C115" s="6">
         <f t="shared" si="11"/>
-        <v>278256056.47503877</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
+        <v>271645612.48707116</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <f t="shared" si="7"/>
-        <v>438601796.74682266</v>
+        <v>11986793504.847744</v>
       </c>
       <c r="C116" s="6">
         <f t="shared" si="11"/>
-        <v>280256056.47503877</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>273645612.48707116</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <f t="shared" si="7"/>
-        <v>445007814.71429086</v>
+        <v>12588233180.090132</v>
       </c>
       <c r="C117" s="6">
         <f t="shared" si="11"/>
-        <v>282256056.47503877</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
+        <v>275645612.48707116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
         <f t="shared" si="7"/>
-        <v>451477892.86143374</v>
+        <v>13219744839.094639</v>
       </c>
       <c r="C118" s="6">
         <f t="shared" si="11"/>
-        <v>284256056.47503877</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
+        <v>277645612.48707116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
         <f t="shared" si="7"/>
-        <v>458012671.79004806</v>
+        <v>13882832081.049372</v>
       </c>
       <c r="C119" s="6">
         <f t="shared" si="11"/>
-        <v>286256056.47503877</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
+        <v>279645612.48707116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
         <f t="shared" si="7"/>
-        <v>464612798.50794852</v>
+        <v>14579073685.101841</v>
       </c>
       <c r="B120" s="6">
         <v>10</v>
       </c>
       <c r="C120" s="6">
         <f>(C119+F$2)*D120</f>
-        <v>299786298.73404032</v>
+        <v>291503208.92411864</v>
       </c>
       <c r="D120" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F120" s="2">
+        <f>A120/C120</f>
+        <v>50.013424342429545</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
         <f t="shared" si="7"/>
-        <v>471278926.49302799</v>
+        <v>15310127369.356934</v>
       </c>
       <c r="C121" s="6">
         <f>C120+F$2</f>
-        <v>301786298.73404032</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
+        <v>293503208.92411864</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <f t="shared" si="7"/>
-        <v>478011715.75795829</v>
+        <v>16077733737.824781</v>
       </c>
       <c r="C122" s="6">
         <f t="shared" ref="C122:C131" si="12">C121+F$2</f>
-        <v>303786298.73404032</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
+        <v>295503208.92411864</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <f t="shared" si="7"/>
-        <v>484811832.91553789</v>
+        <v>16883720424.716021</v>
       </c>
       <c r="C123" s="6">
         <f t="shared" si="12"/>
-        <v>305786298.73404032</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
+        <v>297503208.92411864</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
         <f t="shared" si="7"/>
-        <v>491679951.24469328</v>
+        <v>17730006445.951824</v>
       </c>
       <c r="C124" s="6">
         <f t="shared" si="12"/>
-        <v>307786298.73404032</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
+        <v>299503208.92411864</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
         <f t="shared" si="7"/>
-        <v>498616750.75714022</v>
+        <v>18618606768.249416</v>
       </c>
       <c r="C125" s="6">
         <f t="shared" si="12"/>
-        <v>309786298.73404032</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
+        <v>301503208.92411864</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
         <f t="shared" si="7"/>
-        <v>505622918.26471162</v>
+        <v>19551637106.661888</v>
       </c>
       <c r="C126" s="6">
         <f t="shared" si="12"/>
-        <v>311786298.73404032</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4">
+        <v>303503208.92411864</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
         <f t="shared" si="7"/>
-        <v>512699147.44735873</v>
+        <v>20531318961.994984</v>
       </c>
       <c r="C127" s="6">
         <f t="shared" si="12"/>
-        <v>313786298.73404032</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
+        <v>305503208.92411864</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
         <f t="shared" si="7"/>
-        <v>519846138.92183232</v>
+        <v>21559984910.094734</v>
       </c>
       <c r="C128" s="6">
         <f t="shared" si="12"/>
-        <v>315786298.73404032</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
+        <v>307503208.92411864</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
         <f t="shared" si="7"/>
-        <v>527064600.31105065</v>
+        <v>22640084155.599472</v>
       </c>
       <c r="C129" s="6">
         <f t="shared" si="12"/>
-        <v>317786298.73404032</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4">
+        <v>309503208.92411864</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
         <f t="shared" si="7"/>
-        <v>534355246.31416118</v>
+        <v>23774188363.379448</v>
       </c>
       <c r="C130" s="6">
         <f t="shared" si="12"/>
-        <v>319786298.73404032</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
+        <v>311503208.92411864</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
         <f t="shared" si="7"/>
-        <v>541718798.77730274</v>
+        <v>24964997781.54842</v>
       </c>
       <c r="C131" s="6">
         <f t="shared" si="12"/>
-        <v>321786298.73404032</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
+        <v>313503208.92411864</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
         <f t="shared" si="7"/>
-        <v>549155986.7650758</v>
+        <v>26215347670.625843</v>
       </c>
       <c r="B132" s="6">
         <v>11</v>
       </c>
       <c r="C132" s="6">
         <f>(C131+F$2)*D132</f>
-        <v>336737750.68340194</v>
+        <v>326545821.23646277</v>
       </c>
       <c r="D132" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F132" s="2">
+        <f>A132/C132</f>
+        <v>80.280762961111151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
         <f t="shared" ref="A133:A168" si="13">(A132+F$2)*G$2</f>
-        <v>556667546.63272655</v>
+        <v>27528215054.157135</v>
       </c>
       <c r="C133" s="6">
         <f>C132+F$2</f>
-        <v>338737750.68340194</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
+        <v>328545821.23646277</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
         <f t="shared" si="13"/>
-        <v>564254222.09905386</v>
+        <v>28906725806.864994</v>
       </c>
       <c r="C134" s="6">
         <f t="shared" ref="C134:C143" si="14">C133+F$2</f>
-        <v>340737750.68340194</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
+        <v>330545821.23646277</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
         <f t="shared" si="13"/>
-        <v>571916764.3200444</v>
+        <v>30354162097.208244</v>
       </c>
       <c r="C135" s="6">
         <f t="shared" si="14"/>
-        <v>342737750.68340194</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
+        <v>332545821.23646277</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
         <f t="shared" si="13"/>
-        <v>579655931.9632448</v>
+        <v>31873970202.068657</v>
       </c>
       <c r="C136" s="6">
         <f t="shared" si="14"/>
-        <v>344737750.68340194</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
+        <v>334545821.23646277</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
         <f t="shared" si="13"/>
-        <v>587472491.28287721</v>
+        <v>33469768712.172092</v>
       </c>
       <c r="C137" s="6">
         <f t="shared" si="14"/>
-        <v>346737750.68340194</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
+        <v>336545821.23646277</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
         <f t="shared" si="13"/>
-        <v>595367216.19570601</v>
+        <v>35145357147.780701</v>
       </c>
       <c r="C138" s="6">
         <f t="shared" si="14"/>
-        <v>348737750.68340194</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
+        <v>338545821.23646277</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
         <f t="shared" si="13"/>
-        <v>603340888.35766304</v>
+        <v>36904725005.169739</v>
       </c>
       <c r="C139" s="6">
         <f t="shared" si="14"/>
-        <v>350737750.68340194</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
+        <v>340545821.23646277</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
         <f t="shared" si="13"/>
-        <v>611394297.24123967</v>
+        <v>38752061255.42823</v>
       </c>
       <c r="C140" s="6">
         <f t="shared" si="14"/>
-        <v>352737750.68340194</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
+        <v>342545821.23646277</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
         <f t="shared" si="13"/>
-        <v>619528240.21365201</v>
+        <v>40691764318.199646</v>
       </c>
       <c r="C141" s="6">
         <f t="shared" si="14"/>
-        <v>354737750.68340194</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
+        <v>344545821.23646277</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
         <f t="shared" si="13"/>
-        <v>627743522.61578858</v>
+        <v>42728452534.109627</v>
       </c>
       <c r="C142" s="6">
         <f t="shared" si="14"/>
-        <v>356737750.68340194</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
+        <v>346545821.23646277</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
         <f t="shared" si="13"/>
-        <v>636040957.84194648</v>
+        <v>44866975160.815109</v>
       </c>
       <c r="C143" s="6">
         <f t="shared" si="14"/>
-        <v>358737750.68340194</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
+        <v>348545821.23646277</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
         <f t="shared" si="13"/>
-        <v>644421367.42036593</v>
+        <v>47112423918.855865</v>
       </c>
       <c r="B144" s="6">
         <v>12</v>
       </c>
       <c r="C144" s="6">
         <f>(C143+F$2)*D144</f>
-        <v>375167260.710738</v>
+        <v>362814924.97973895</v>
       </c>
       <c r="D144" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F144" s="2">
+        <f>A144/C144</f>
+        <v>129.85249689352446</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
         <f t="shared" si="13"/>
-        <v>652885581.09456956</v>
+        <v>49470145114.79866</v>
       </c>
       <c r="C145" s="6">
         <f>C144+F$2</f>
-        <v>377167260.710738</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
+        <v>364814924.97973895</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
         <f t="shared" si="13"/>
-        <v>661434436.90551531</v>
+        <v>51945752370.538597</v>
       </c>
       <c r="C146" s="6">
         <f t="shared" ref="C146:C155" si="15">C145+F$2</f>
-        <v>379167260.710738</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
+        <v>366814924.97973895</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
         <f t="shared" si="13"/>
-        <v>670068781.27457047</v>
+        <v>54545139989.065529</v>
       </c>
       <c r="C147" s="6">
         <f t="shared" si="15"/>
-        <v>381167260.710738</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
+        <v>368814924.97973895</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
         <f t="shared" si="13"/>
-        <v>678789469.08731616</v>
+        <v>57274496988.518806</v>
       </c>
       <c r="C148" s="6">
         <f t="shared" si="15"/>
-        <v>383167260.710738</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
+        <v>370814924.97973895</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
         <f t="shared" si="13"/>
-        <v>687597363.7781893</v>
+        <v>60140321837.944748</v>
       </c>
       <c r="C149" s="6">
         <f t="shared" si="15"/>
-        <v>385167260.710738</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
+        <v>372814924.97973895</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
         <f t="shared" si="13"/>
-        <v>696493337.41597116</v>
+        <v>63149437929.841988</v>
       </c>
       <c r="C150" s="6">
         <f t="shared" si="15"/>
-        <v>387167260.710738</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
+        <v>374814924.97973895</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
         <f t="shared" si="13"/>
-        <v>705478270.79013085</v>
+        <v>66309009826.334091</v>
       </c>
       <c r="C151" s="6">
         <f t="shared" si="15"/>
-        <v>389167260.710738</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
+        <v>376814924.97973895</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
         <f t="shared" si="13"/>
-        <v>714553053.49803221</v>
+        <v>69626560317.650803</v>
       </c>
       <c r="C152" s="6">
         <f t="shared" si="15"/>
-        <v>391167260.710738</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
+        <v>378814924.97973895</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
         <f t="shared" si="13"/>
-        <v>723718584.03301251</v>
+        <v>73109988333.53334</v>
       </c>
       <c r="C153" s="6">
         <f t="shared" si="15"/>
-        <v>393167260.710738</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
+        <v>380814924.97973895</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
         <f t="shared" si="13"/>
-        <v>732975769.87334263</v>
+        <v>76767587750.210007</v>
       </c>
       <c r="C154" s="6">
         <f t="shared" si="15"/>
-        <v>395167260.710738</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
+        <v>382814924.97973895</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
         <f t="shared" si="13"/>
-        <v>742325527.57207608</v>
+        <v>80608067137.720505</v>
       </c>
       <c r="C155" s="6">
         <f t="shared" si="15"/>
-        <v>397167260.710738</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
+        <v>384814924.97973895</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
         <f t="shared" si="13"/>
-        <v>751768782.8477968</v>
+        <v>84640570494.606537</v>
       </c>
       <c r="B156" s="6">
         <v>13</v>
       </c>
       <c r="C156" s="6">
         <f>(C155+F$2)*D156</f>
-        <v>415133951.13916755</v>
+        <v>400353447.35402977</v>
       </c>
       <c r="D156" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F156" s="2">
+        <f>A156/C156</f>
+        <v>211.41461639459661</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
         <f t="shared" si="13"/>
-        <v>761306470.67627478</v>
+        <v>88874699019.336868</v>
       </c>
       <c r="C157" s="6">
         <f>C156+F$2</f>
-        <v>417133951.13916755</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
+        <v>402353447.35402977</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
         <f t="shared" si="13"/>
-        <v>770939535.38303757</v>
+        <v>93320533970.303711</v>
       </c>
       <c r="C158" s="6">
         <f t="shared" ref="C158:C167" si="16">C157+F$2</f>
-        <v>419133951.13916755</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
+        <v>404353447.35402977</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
         <f t="shared" si="13"/>
-        <v>780668930.7368679</v>
+        <v>97988660668.818893</v>
       </c>
       <c r="C159" s="6">
         <f t="shared" si="16"/>
-        <v>421133951.13916755</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
+        <v>406353447.35402977</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
         <f t="shared" si="13"/>
-        <v>790495620.04423654</v>
+        <v>102890193702.25984</v>
       </c>
       <c r="C160" s="6">
         <f t="shared" si="16"/>
-        <v>423133951.13916755</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
+        <v>408353447.35402977</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
         <f t="shared" si="13"/>
-        <v>800420576.24467885</v>
+        <v>108036803387.37283</v>
       </c>
       <c r="C161" s="6">
         <f t="shared" si="16"/>
-        <v>425133951.13916755</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4">
+        <v>410353447.35402977</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
         <f t="shared" si="13"/>
-        <v>810444782.00712562</v>
+        <v>113440743556.74149</v>
       </c>
       <c r="C162" s="6">
         <f t="shared" si="16"/>
-        <v>427133951.13916755</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
+        <v>412353447.35402977</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
         <f t="shared" si="13"/>
-        <v>820569229.82719684</v>
+        <v>119114880734.57857</v>
       </c>
       <c r="C163" s="6">
         <f t="shared" si="16"/>
-        <v>429133951.13916755</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4">
+        <v>414353447.35402977</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
         <f t="shared" si="13"/>
-        <v>830794922.12546885</v>
+        <v>125072724771.3075</v>
       </c>
       <c r="C164" s="6">
         <f t="shared" si="16"/>
-        <v>431133951.13916755</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
+        <v>416353447.35402977</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
         <f t="shared" si="13"/>
-        <v>841122871.34672356</v>
+        <v>131328461009.87288</v>
       </c>
       <c r="C165" s="6">
         <f t="shared" si="16"/>
-        <v>433133951.13916755</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4">
+        <v>418353447.35402977</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
         <f t="shared" si="13"/>
-        <v>851554100.0601908</v>
+        <v>137896984060.36652</v>
       </c>
       <c r="C166" s="6">
         <f t="shared" si="16"/>
-        <v>435133951.13916755</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
+        <v>420353447.35402977</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
         <f t="shared" si="13"/>
-        <v>862089641.06079268</v>
+        <v>144793933263.38486</v>
       </c>
       <c r="C167" s="6">
         <f t="shared" si="16"/>
-        <v>437133951.13916755</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
+        <v>422353447.35402977</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
         <f t="shared" si="13"/>
-        <v>872730537.47140062</v>
+        <v>152035729926.55411</v>
       </c>
       <c r="B168" s="6">
         <v>14</v>
       </c>
       <c r="C168" s="6">
         <f>(C167+F$2)*D168</f>
-        <v>456699309.18473428</v>
+        <v>439205818.01142079</v>
       </c>
       <c r="D168" s="2">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F168" s="2">
+        <f>A168/C168</f>
+        <v>346.1605554655942</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
         <f t="shared" ref="A169:A180" si="17">(A168+F$2)*G$2</f>
-        <v>883477842.84611464</v>
+        <v>159639616422.88181</v>
       </c>
       <c r="C169" s="6">
         <f>C168+F$2</f>
-        <v>458699309.18473428</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
+        <v>441205818.01142079</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
         <f t="shared" si="17"/>
-        <v>894332621.27457583</v>
+        <v>167623697244.02591</v>
       </c>
       <c r="C170" s="6">
         <f t="shared" ref="C170:C179" si="18">C169+F$2</f>
-        <v>460699309.18473428</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
+        <v>443205818.01142079</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
         <f t="shared" si="17"/>
-        <v>905295947.48732162</v>
+        <v>176006982106.2272</v>
       </c>
       <c r="C171" s="6">
         <f t="shared" si="18"/>
-        <v>462699309.18473428</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
+        <v>445205818.01142079</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="6">
         <f t="shared" si="17"/>
-        <v>916368906.9621948</v>
+        <v>184809431211.53857</v>
       </c>
       <c r="C172" s="6">
         <f t="shared" si="18"/>
-        <v>464699309.18473428</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
+        <v>447205818.01142079</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="6">
         <f t="shared" si="17"/>
-        <v>927552596.03181672</v>
+        <v>194052002772.11551</v>
       </c>
       <c r="C173" s="6">
         <f t="shared" si="18"/>
-        <v>466699309.18473428</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
+        <v>449205818.01142079</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="6">
         <f t="shared" si="17"/>
-        <v>938848121.99213493</v>
+        <v>203756702910.72128</v>
       </c>
       <c r="C174" s="6">
         <f t="shared" si="18"/>
-        <v>468699309.18473428</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
+        <v>451205818.01142079</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="6">
         <f t="shared" si="17"/>
-        <v>950256603.21205628</v>
+        <v>213946638056.25735</v>
       </c>
       <c r="C175" s="6">
         <f t="shared" si="18"/>
-        <v>470699309.18473428</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4">
+        <v>453205818.01142079</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="6">
         <f t="shared" si="17"/>
-        <v>961779169.24417686</v>
+        <v>224646069959.07022</v>
       </c>
       <c r="C176" s="6">
         <f t="shared" si="18"/>
-        <v>472699309.18473428</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6">
+        <v>455205818.01142079</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="6">
         <f t="shared" si="17"/>
-        <v>973416960.93661869</v>
+        <v>235880473457.02374</v>
       </c>
       <c r="C177" s="6">
         <f t="shared" si="18"/>
-        <v>474699309.18473428</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6">
+        <v>457205818.01142079</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="6">
         <f t="shared" si="17"/>
-        <v>985171130.54598486</v>
+        <v>247676597129.87494</v>
       </c>
       <c r="C178" s="6">
         <f t="shared" si="18"/>
-        <v>476699309.18473428</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
+        <v>459205818.01142079</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="6">
         <f t="shared" si="17"/>
-        <v>997042841.85144472</v>
+        <v>260062526986.36868</v>
       </c>
       <c r="C179" s="6">
         <f t="shared" si="18"/>
-        <v>478699309.18473428</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
+        <v>461205818.01142079</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="6">
         <f t="shared" si="17"/>
-        <v>1009033270.2699592</v>
+        <v>273067753335.68713</v>
       </c>
       <c r="B180" s="6">
         <v>15</v>
       </c>
       <c r="C180" s="6">
         <f>(C179+F$2)*D180</f>
-        <v>499927281.55212367</v>
+        <v>479418021.64182049</v>
       </c>
       <c r="D180" s="2">
-        <v>1.04</v>
-      </c>
-      <c r="F180" s="6" t="s">
-        <v>30</v>
+        <f>$H$2</f>
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="F180" s="2">
+        <f>A180/C180</f>
+        <v>569.58174496765093</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>